<commit_message>
New results and figures in pdf
</commit_message>
<xml_diff>
--- a/resources/historical_rulesv1.xlsx
+++ b/resources/historical_rulesv1.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -50,22 +50,89 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -358,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:K115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,7 +493,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>frozenset({'IBM DB2'})</t>
+          <t>frozenset({'SAP SQL Anywhere'})</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -435,25 +502,27 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="E2" t="n">
-        <v>0.02538071065989848</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5555555555555556</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>15.63492063492063</v>
+        <v>21.66666666666666</v>
       </c>
       <c r="H2" t="n">
-        <v>0.02375737586642274</v>
-      </c>
-      <c r="I2" t="n">
-        <v>2.17005076142132</v>
+        <v>0.04402366863905326</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
       <c r="J2" t="n">
         <v>1</v>
@@ -470,29 +539,31 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>frozenset({'IBM DB2'})</t>
+          <t>frozenset({'SAP SQL Anywhere'})</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="D3" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="E3" t="n">
-        <v>0.02538071065989848</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7142857142857142</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>15.63492063492063</v>
+        <v>21.66666666666666</v>
       </c>
       <c r="H3" t="n">
-        <v>0.02375737586642274</v>
-      </c>
-      <c r="I3" t="n">
-        <v>3.340101522842638</v>
+        <v>0.04402366863905326</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
       <c r="J3" t="n">
         <v>1</v>
@@ -504,36 +575,34 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>frozenset({'Informix'})</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>frozenset({'Oracle'})</t>
-        </is>
-      </c>
       <c r="C4" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="E4" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>0.8333333333333333</v>
       </c>
       <c r="G4" t="n">
-        <v>7.880000000000001</v>
+        <v>14.77272727272727</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0398876549254039</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>0.02390532544378698</v>
+      </c>
+      <c r="I4" t="n">
+        <v>5.661538461538459</v>
       </c>
       <c r="J4" t="n">
         <v>1</v>
@@ -545,34 +614,34 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>frozenset({'IBM DB2'})</t>
+          <t>frozenset({'Informix'})</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="D5" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="E5" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F5" t="n">
-        <v>0.36</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="G5" t="n">
-        <v>7.88</v>
+        <v>14.77272727272727</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0398876549254039</v>
+        <v>0.02390532544378698</v>
       </c>
       <c r="I5" t="n">
-        <v>1.491116751269036</v>
+        <v>1.776923076923077</v>
       </c>
       <c r="J5" t="n">
         <v>1</v>
@@ -584,34 +653,34 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>frozenset({'MS SQL Server'})</t>
+          <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>frozenset({'SQLite'})</t>
+          <t>frozenset({'SAP SQL Anywhere'})</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.04060913705583756</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="D6" t="n">
-        <v>0.08121827411167512</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="E6" t="n">
-        <v>0.02538071065989848</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="F6" t="n">
-        <v>0.625</v>
+        <v>0.5454545454545455</v>
       </c>
       <c r="G6" t="n">
-        <v>7.695312500000001</v>
+        <v>11.81818181818182</v>
       </c>
       <c r="H6" t="n">
-        <v>0.02208250663505888</v>
+        <v>0.02816568047337278</v>
       </c>
       <c r="I6" t="n">
-        <v>2.450084602368866</v>
+        <v>2.098461538461539</v>
       </c>
       <c r="J6" t="n">
         <v>1</v>
@@ -623,34 +692,34 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>frozenset({'SQLite'})</t>
+          <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>frozenset({'MS SQL Server'})</t>
+          <t>frozenset({'SAP Adaptive Server'})</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.08121827411167512</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="D7" t="n">
-        <v>0.04060913705583756</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="E7" t="n">
-        <v>0.02538071065989848</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3125</v>
+        <v>0.5454545454545455</v>
       </c>
       <c r="G7" t="n">
-        <v>7.695312500000001</v>
+        <v>11.81818181818182</v>
       </c>
       <c r="H7" t="n">
-        <v>0.02208250663505888</v>
+        <v>0.02816568047337278</v>
       </c>
       <c r="I7" t="n">
-        <v>1.395477618827873</v>
+        <v>2.098461538461539</v>
       </c>
       <c r="J7" t="n">
         <v>1</v>
@@ -662,34 +731,34 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>frozenset({'MS SQL Server'})</t>
+          <t>frozenset({'SAP Adaptive Server'})</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.04060913705583756</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="E8" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8750000000000001</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G8" t="n">
-        <v>6.895000000000001</v>
+        <v>11.81818181818182</v>
       </c>
       <c r="H8" t="n">
-        <v>0.030379551135046</v>
+        <v>0.02816568047337278</v>
       </c>
       <c r="I8" t="n">
-        <v>6.984771573604067</v>
+        <v>2.83076923076923</v>
       </c>
       <c r="J8" t="n">
         <v>1</v>
@@ -701,34 +770,34 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'SAP SQL Anywhere'})</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>frozenset({'MS SQL Server'})</t>
+          <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="D9" t="n">
-        <v>0.04060913705583756</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="E9" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="F9" t="n">
-        <v>0.28</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G9" t="n">
-        <v>6.895000000000001</v>
+        <v>11.81818181818182</v>
       </c>
       <c r="H9" t="n">
-        <v>0.030379551135046</v>
+        <v>0.02816568047337278</v>
       </c>
       <c r="I9" t="n">
-        <v>1.33248730964467</v>
+        <v>2.83076923076923</v>
       </c>
       <c r="J9" t="n">
         <v>1</v>
@@ -740,34 +809,34 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>frozenset({'SAP Adaptive Server'})</t>
+          <t>frozenset({'SQLite'})</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'Informix'})</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.08717948717948718</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="E10" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F10" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.2941176470588235</v>
       </c>
       <c r="G10" t="n">
-        <v>6.754285714285714</v>
+        <v>9.558823529411764</v>
       </c>
       <c r="H10" t="n">
-        <v>0.02594758947666779</v>
+        <v>0.0229585798816568</v>
       </c>
       <c r="I10" t="n">
-        <v>6.111675126903551</v>
+        <v>1.373076923076923</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
@@ -779,34 +848,34 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'Informix'})</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>frozenset({'SAP Adaptive Server'})</t>
+          <t>frozenset({'SQLite'})</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="D11" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.08717948717948718</v>
       </c>
       <c r="E11" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F11" t="n">
-        <v>0.24</v>
+        <v>0.8333333333333333</v>
       </c>
       <c r="G11" t="n">
-        <v>6.754285714285714</v>
+        <v>9.558823529411764</v>
       </c>
       <c r="H11" t="n">
-        <v>0.02594758947666779</v>
+        <v>0.0229585798816568</v>
       </c>
       <c r="I11" t="n">
-        <v>1.269035532994924</v>
+        <v>5.476923076923074</v>
       </c>
       <c r="J11" t="n">
         <v>1</v>
@@ -818,34 +887,34 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>frozenset({'MS Access'})</t>
+          <t>frozenset({'MS SQL Server_Microsoft Azure SQL Database'})</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="D12" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.05128205128205128</v>
       </c>
       <c r="E12" t="n">
-        <v>0.02538071065989848</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="G12" t="n">
-        <v>6.566666666666666</v>
+        <v>8.863636363636363</v>
       </c>
       <c r="H12" t="n">
-        <v>0.02151562781828957</v>
+        <v>0.02274819197896121</v>
       </c>
       <c r="I12" t="n">
-        <v>1.211928934010152</v>
+        <v>1.739316239316239</v>
       </c>
       <c r="J12" t="n">
         <v>1</v>
@@ -857,34 +926,34 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>frozenset({'MS Access'})</t>
+          <t>frozenset({'MS SQL Server_Microsoft Azure SQL Database'})</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.05128205128205128</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="E13" t="n">
-        <v>0.02538071065989848</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F13" t="n">
-        <v>0.8333333333333333</v>
+        <v>0.5</v>
       </c>
       <c r="G13" t="n">
-        <v>6.566666666666666</v>
+        <v>8.863636363636363</v>
       </c>
       <c r="H13" t="n">
-        <v>0.02151562781828957</v>
+        <v>0.02274819197896121</v>
       </c>
       <c r="I13" t="n">
-        <v>5.238578680203043</v>
+        <v>1.887179487179487</v>
       </c>
       <c r="J13" t="n">
         <v>1</v>
@@ -896,34 +965,34 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>frozenset({'MS Access'})</t>
+          <t>frozenset({'HyperSQL'})</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'Informix'})</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.1384615384615385</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="E14" t="n">
-        <v>0.02538071065989848</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="F14" t="n">
-        <v>0.8333333333333333</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="G14" t="n">
-        <v>5.295698924731182</v>
+        <v>7.222222222222221</v>
       </c>
       <c r="H14" t="n">
-        <v>0.02058800793630344</v>
+        <v>0.02650887573964497</v>
       </c>
       <c r="I14" t="n">
-        <v>5.055837563451774</v>
+        <v>1.246153846153846</v>
       </c>
       <c r="J14" t="n">
         <v>1</v>
@@ -935,34 +1004,36 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'Informix'})</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>frozenset({'MS Access'})</t>
+          <t>frozenset({'HyperSQL'})</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="D15" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.1384615384615385</v>
       </c>
       <c r="E15" t="n">
-        <v>0.02538071065989848</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1612903225806452</v>
+        <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>5.295698924731182</v>
+        <v>7.222222222222221</v>
       </c>
       <c r="H15" t="n">
-        <v>0.02058800793630344</v>
-      </c>
-      <c r="I15" t="n">
-        <v>1.155993752440453</v>
+        <v>0.02650887573964497</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
       <c r="J15" t="n">
         <v>1</v>
@@ -974,7 +1045,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -983,25 +1054,25 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.182741116751269</v>
+        <v>0.1435897435897436</v>
       </c>
       <c r="D16" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="E16" t="n">
-        <v>0.04060913705583756</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="F16" t="n">
-        <v>0.2222222222222222</v>
+        <v>0.3928571428571429</v>
       </c>
       <c r="G16" t="n">
-        <v>4.864197530864198</v>
+        <v>6.964285714285715</v>
       </c>
       <c r="H16" t="n">
-        <v>0.03226055811796233</v>
+        <v>0.048310322156476</v>
       </c>
       <c r="I16" t="n">
-        <v>1.226976069615664</v>
+        <v>1.554147812971342</v>
       </c>
       <c r="J16" t="n">
         <v>1</v>
@@ -1018,29 +1089,31 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="D17" t="n">
-        <v>0.182741116751269</v>
+        <v>0.1435897435897436</v>
       </c>
       <c r="E17" t="n">
-        <v>0.04060913705583756</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="F17" t="n">
-        <v>0.8888888888888888</v>
+        <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>4.864197530864198</v>
+        <v>6.964285714285714</v>
       </c>
       <c r="H17" t="n">
-        <v>0.03226055811796233</v>
-      </c>
-      <c r="I17" t="n">
-        <v>7.355329949238575</v>
+        <v>0.048310322156476</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
       <c r="J17" t="n">
         <v>1</v>
@@ -1052,34 +1125,34 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'MS SQL Server_Microsoft Azure SQL Database'})</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>frozenset({'MS SQL Server'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.182741116751269</v>
+        <v>0.05128205128205128</v>
       </c>
       <c r="D18" t="n">
-        <v>0.04060913705583756</v>
+        <v>0.1435897435897436</v>
       </c>
       <c r="E18" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="F18" t="n">
-        <v>0.1944444444444445</v>
+        <v>0.9000000000000001</v>
       </c>
       <c r="G18" t="n">
-        <v>4.788194444444446</v>
+        <v>6.267857142857144</v>
       </c>
       <c r="H18" t="n">
-        <v>0.02811203586796877</v>
+        <v>0.03879026955950033</v>
       </c>
       <c r="I18" t="n">
-        <v>1.190967967792753</v>
+        <v>8.564102564102576</v>
       </c>
       <c r="J18" t="n">
         <v>1</v>
@@ -1091,34 +1164,34 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>frozenset({'MS SQL Server'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'MS SQL Server_Microsoft Azure SQL Database'})</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.04060913705583756</v>
+        <v>0.1435897435897436</v>
       </c>
       <c r="D19" t="n">
-        <v>0.182741116751269</v>
+        <v>0.05128205128205128</v>
       </c>
       <c r="E19" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="F19" t="n">
-        <v>0.8750000000000001</v>
+        <v>0.3214285714285715</v>
       </c>
       <c r="G19" t="n">
-        <v>4.788194444444446</v>
+        <v>6.267857142857143</v>
       </c>
       <c r="H19" t="n">
-        <v>0.02811203586796877</v>
+        <v>0.03879026955950033</v>
       </c>
       <c r="I19" t="n">
-        <v>6.538071065989854</v>
+        <v>1.398110661268556</v>
       </c>
       <c r="J19" t="n">
         <v>1</v>
@@ -1130,34 +1203,34 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>frozenset({'MS Access'})</t>
+          <t>frozenset({'SAP Adaptive Server'})</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.182741116751269</v>
+        <v>0.1435897435897436</v>
       </c>
       <c r="D20" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="E20" t="n">
-        <v>0.02538071065989848</v>
+        <v>0.04102564102564103</v>
       </c>
       <c r="F20" t="n">
-        <v>0.1388888888888889</v>
+        <v>0.2857142857142858</v>
       </c>
       <c r="G20" t="n">
-        <v>4.560185185185185</v>
+        <v>6.190476190476191</v>
       </c>
       <c r="H20" t="n">
-        <v>0.01981499136798165</v>
+        <v>0.03439842209072978</v>
       </c>
       <c r="I20" t="n">
-        <v>1.125921074177174</v>
+        <v>1.335384615384615</v>
       </c>
       <c r="J20" t="n">
         <v>1</v>
@@ -1169,34 +1242,34 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>frozenset({'MS Access'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'SAP SQL Anywhere'})</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.1435897435897436</v>
       </c>
       <c r="D21" t="n">
-        <v>0.182741116751269</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="E21" t="n">
-        <v>0.02538071065989848</v>
+        <v>0.04102564102564103</v>
       </c>
       <c r="F21" t="n">
-        <v>0.8333333333333333</v>
+        <v>0.2857142857142858</v>
       </c>
       <c r="G21" t="n">
-        <v>4.560185185185185</v>
+        <v>6.190476190476191</v>
       </c>
       <c r="H21" t="n">
-        <v>0.01981499136798165</v>
+        <v>0.03439842209072978</v>
       </c>
       <c r="I21" t="n">
-        <v>4.903553299492383</v>
+        <v>1.335384615384615</v>
       </c>
       <c r="J21" t="n">
         <v>1</v>
@@ -1208,34 +1281,34 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'SAP SQL Anywhere'})</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>frozenset({'SAP Adaptive Server'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="D22" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.1435897435897436</v>
       </c>
       <c r="E22" t="n">
-        <v>0.02538071065989848</v>
+        <v>0.04102564102564103</v>
       </c>
       <c r="F22" t="n">
-        <v>0.1612903225806452</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="G22" t="n">
-        <v>4.539170506912442</v>
+        <v>6.190476190476191</v>
       </c>
       <c r="H22" t="n">
-        <v>0.0197892241490376</v>
+        <v>0.03439842209072978</v>
       </c>
       <c r="I22" t="n">
-        <v>1.149941429129246</v>
+        <v>7.707692307692305</v>
       </c>
       <c r="J22" t="n">
         <v>1</v>
@@ -1252,29 +1325,29 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="D23" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.1435897435897436</v>
       </c>
       <c r="E23" t="n">
-        <v>0.02538071065989848</v>
+        <v>0.04102564102564103</v>
       </c>
       <c r="F23" t="n">
-        <v>0.7142857142857142</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="G23" t="n">
-        <v>4.539170506912442</v>
+        <v>6.190476190476191</v>
       </c>
       <c r="H23" t="n">
-        <v>0.0197892241490376</v>
+        <v>0.03439842209072978</v>
       </c>
       <c r="I23" t="n">
-        <v>2.949238578680202</v>
+        <v>7.707692307692305</v>
       </c>
       <c r="J23" t="n">
         <v>1</v>
@@ -1291,29 +1364,29 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'HyperSQL'})</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="D24" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.1384615384615385</v>
       </c>
       <c r="E24" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="F24" t="n">
-        <v>0.6666666666666667</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="G24" t="n">
-        <v>4.236559139784947</v>
+        <v>5.909090909090909</v>
       </c>
       <c r="H24" t="n">
-        <v>0.02326779870648561</v>
+        <v>0.03834319526627219</v>
       </c>
       <c r="I24" t="n">
-        <v>2.527918781725889</v>
+        <v>4.73846153846154</v>
       </c>
       <c r="J24" t="n">
         <v>1</v>
@@ -1325,7 +1398,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'HyperSQL'})</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1334,25 +1407,25 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.1384615384615385</v>
       </c>
       <c r="D25" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="E25" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="F25" t="n">
-        <v>0.1935483870967742</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="G25" t="n">
-        <v>4.236559139784946</v>
+        <v>5.909090909090908</v>
       </c>
       <c r="H25" t="n">
-        <v>0.02326779870648561</v>
+        <v>0.03834319526627219</v>
       </c>
       <c r="I25" t="n">
-        <v>1.183350253807107</v>
+        <v>1.415384615384615</v>
       </c>
       <c r="J25" t="n">
         <v>1</v>
@@ -1364,34 +1437,34 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'Informix'})</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>frozenset({'MS SQL Server'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="D26" t="n">
-        <v>0.04060913705583756</v>
+        <v>0.1435897435897436</v>
       </c>
       <c r="E26" t="n">
-        <v>0.02538071065989848</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F26" t="n">
-        <v>0.1612903225806452</v>
+        <v>0.8333333333333333</v>
       </c>
       <c r="G26" t="n">
-        <v>3.971774193548387</v>
+        <v>5.803571428571429</v>
       </c>
       <c r="H26" t="n">
-        <v>0.01899044036177176</v>
+        <v>0.02122287968441815</v>
       </c>
       <c r="I26" t="n">
-        <v>1.14388910581804</v>
+        <v>5.138461538461536</v>
       </c>
       <c r="J26" t="n">
         <v>1</v>
@@ -1403,34 +1476,34 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>frozenset({'MS SQL Server'})</t>
+          <t>frozenset({'MS Access'})</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.04060913705583756</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="D27" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.1435897435897436</v>
       </c>
       <c r="E27" t="n">
-        <v>0.02538071065989848</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F27" t="n">
-        <v>0.625</v>
+        <v>0.8333333333333333</v>
       </c>
       <c r="G27" t="n">
-        <v>3.971774193548387</v>
+        <v>5.803571428571429</v>
       </c>
       <c r="H27" t="n">
-        <v>0.01899044036177176</v>
+        <v>0.02122287968441815</v>
       </c>
       <c r="I27" t="n">
-        <v>2.247038917089678</v>
+        <v>5.138461538461536</v>
       </c>
       <c r="J27" t="n">
         <v>1</v>
@@ -1442,34 +1515,34 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>frozenset({'SAP Adaptive Server'})</t>
+          <t>frozenset({'Informix'})</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.182741116751269</v>
+        <v>0.1435897435897436</v>
       </c>
       <c r="D28" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="E28" t="n">
-        <v>0.02538071065989848</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F28" t="n">
-        <v>0.1388888888888889</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="G28" t="n">
-        <v>3.908730158730159</v>
+        <v>5.803571428571428</v>
       </c>
       <c r="H28" t="n">
-        <v>0.01888737148599551</v>
+        <v>0.02122287968441815</v>
       </c>
       <c r="I28" t="n">
-        <v>1.120026199443262</v>
+        <v>1.179933110367893</v>
       </c>
       <c r="J28" t="n">
         <v>1</v>
@@ -1481,34 +1554,34 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>frozenset({'SAP Adaptive Server'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'MS Access'})</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.1435897435897436</v>
       </c>
       <c r="D29" t="n">
-        <v>0.182741116751269</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="E29" t="n">
-        <v>0.02538071065989848</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F29" t="n">
-        <v>0.7142857142857142</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="G29" t="n">
-        <v>3.908730158730158</v>
+        <v>5.803571428571428</v>
       </c>
       <c r="H29" t="n">
-        <v>0.01888737148599551</v>
+        <v>0.02122287968441815</v>
       </c>
       <c r="I29" t="n">
-        <v>2.860406091370558</v>
+        <v>1.179933110367893</v>
       </c>
       <c r="J29" t="n">
         <v>1</v>
@@ -1520,34 +1593,34 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'SQLite'})</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'MS SQL Server_Microsoft Azure SQL Database'})</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.08717948717948718</v>
       </c>
       <c r="D30" t="n">
-        <v>0.182741116751269</v>
+        <v>0.05128205128205128</v>
       </c>
       <c r="E30" t="n">
-        <v>0.08629441624365482</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F30" t="n">
-        <v>0.68</v>
+        <v>0.2941176470588235</v>
       </c>
       <c r="G30" t="n">
-        <v>3.721111111111111</v>
+        <v>5.735294117647059</v>
       </c>
       <c r="H30" t="n">
-        <v>0.06310391919400139</v>
+        <v>0.02117028270874425</v>
       </c>
       <c r="I30" t="n">
-        <v>2.553934010152285</v>
+        <v>1.344017094017094</v>
       </c>
       <c r="J30" t="n">
         <v>1</v>
@@ -1559,34 +1632,34 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'MS SQL Server_Microsoft Azure SQL Database'})</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'SQLite'})</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.182741116751269</v>
+        <v>0.05128205128205128</v>
       </c>
       <c r="D31" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.08717948717948718</v>
       </c>
       <c r="E31" t="n">
-        <v>0.08629441624365482</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F31" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="G31" t="n">
-        <v>3.721111111111111</v>
+        <v>5.735294117647059</v>
       </c>
       <c r="H31" t="n">
-        <v>0.06310391919400139</v>
+        <v>0.02117028270874425</v>
       </c>
       <c r="I31" t="n">
-        <v>1.654288004274646</v>
+        <v>1.825641025641026</v>
       </c>
       <c r="J31" t="n">
         <v>1</v>
@@ -1598,34 +1671,34 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>frozenset({'SQLite'})</t>
+          <t>frozenset({'H2'})</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'Informix'})</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.08121827411167512</v>
+        <v>0.1743589743589744</v>
       </c>
       <c r="D32" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="E32" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="F32" t="n">
-        <v>0.5625</v>
+        <v>0.1764705882352941</v>
       </c>
       <c r="G32" t="n">
-        <v>3.574596774193548</v>
+        <v>5.735294117647059</v>
       </c>
       <c r="H32" t="n">
-        <v>0.03290473859156381</v>
+        <v>0.0254043392504931</v>
       </c>
       <c r="I32" t="n">
-        <v>1.926033357505439</v>
+        <v>1.176923076923077</v>
       </c>
       <c r="J32" t="n">
         <v>1</v>
@@ -1637,34 +1710,36 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>frozenset({'Informix'})</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
           <t>frozenset({'H2'})</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>frozenset({'SQLite'})</t>
-        </is>
-      </c>
       <c r="C33" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="D33" t="n">
-        <v>0.08121827411167512</v>
+        <v>0.1743589743589744</v>
       </c>
       <c r="E33" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="F33" t="n">
-        <v>0.2903225806451613</v>
+        <v>1</v>
       </c>
       <c r="G33" t="n">
-        <v>3.574596774193548</v>
+        <v>5.735294117647059</v>
       </c>
       <c r="H33" t="n">
-        <v>0.03290473859156381</v>
-      </c>
-      <c r="I33" t="n">
-        <v>1.294646977388094</v>
+        <v>0.0254043392504931</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
       <c r="J33" t="n">
         <v>1</v>
@@ -1676,7 +1751,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1685,25 +1760,25 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="D34" t="n">
-        <v>0.08121827411167512</v>
+        <v>0.08717948717948718</v>
       </c>
       <c r="E34" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F34" t="n">
-        <v>0.28</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="G34" t="n">
-        <v>3.447500000000001</v>
+        <v>5.213903743315508</v>
       </c>
       <c r="H34" t="n">
-        <v>0.02522610734623412</v>
+        <v>0.02072320841551611</v>
       </c>
       <c r="I34" t="n">
-        <v>1.276085730400451</v>
+        <v>1.673504273504274</v>
       </c>
       <c r="J34" t="n">
         <v>1</v>
@@ -1720,29 +1795,29 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.08121827411167512</v>
+        <v>0.08717948717948718</v>
       </c>
       <c r="D35" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="E35" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F35" t="n">
-        <v>0.4375000000000001</v>
+        <v>0.2941176470588235</v>
       </c>
       <c r="G35" t="n">
-        <v>3.447500000000001</v>
+        <v>5.213903743315508</v>
       </c>
       <c r="H35" t="n">
-        <v>0.02522610734623412</v>
+        <v>0.02072320841551611</v>
       </c>
       <c r="I35" t="n">
-        <v>1.552171460800902</v>
+        <v>1.336752136752137</v>
       </c>
       <c r="J35" t="n">
         <v>1</v>
@@ -1754,36 +1829,34 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>frozenset({'MS Access'})</t>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'Informix'})</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.1948717948717949</v>
       </c>
       <c r="D36" t="n">
-        <v>0.299492385786802</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="E36" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="F36" t="n">
-        <v>1</v>
+        <v>0.1578947368421053</v>
       </c>
       <c r="G36" t="n">
-        <v>3.338983050847458</v>
+        <v>5.131578947368421</v>
       </c>
       <c r="H36" t="n">
-        <v>0.02133525728568116</v>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>0.02477317554240631</v>
+      </c>
+      <c r="I36" t="n">
+        <v>1.150961538461539</v>
       </c>
       <c r="J36" t="n">
         <v>1</v>
@@ -1795,34 +1868,36 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'Informix'})</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>frozenset({'SAP Adaptive Server'})</t>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.299492385786802</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="D37" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.1948717948717949</v>
       </c>
       <c r="E37" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="F37" t="n">
-        <v>0.1186440677966102</v>
+        <v>1</v>
       </c>
       <c r="G37" t="n">
-        <v>3.338983050847458</v>
+        <v>5.131578947368421</v>
       </c>
       <c r="H37" t="n">
-        <v>0.02489113349996135</v>
-      </c>
-      <c r="I37" t="n">
-        <v>1.094299101913315</v>
+        <v>0.02477317554240631</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
       <c r="J37" t="n">
         <v>1</v>
@@ -1839,31 +1914,29 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'HyperSQL'})</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="D38" t="n">
-        <v>0.299492385786802</v>
+        <v>0.1384615384615385</v>
       </c>
       <c r="E38" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="F38" t="n">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G38" t="n">
-        <v>3.338983050847458</v>
+        <v>4.814814814814814</v>
       </c>
       <c r="H38" t="n">
-        <v>0.02489113349996135</v>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>0.02437869822485207</v>
+      </c>
+      <c r="I38" t="n">
+        <v>2.584615384615384</v>
       </c>
       <c r="J38" t="n">
         <v>1</v>
@@ -1875,36 +1948,34 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>frozenset({'IBM DB2'})</t>
+          <t>frozenset({'HyperSQL'})</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'SAP SQL Anywhere'})</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.1384615384615385</v>
       </c>
       <c r="D39" t="n">
-        <v>0.299492385786802</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="E39" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="F39" t="n">
-        <v>1</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="G39" t="n">
-        <v>3.338983050847458</v>
+        <v>4.814814814814814</v>
       </c>
       <c r="H39" t="n">
-        <v>0.03200288592852173</v>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>0.02437869822485207</v>
+      </c>
+      <c r="I39" t="n">
+        <v>1.226373626373626</v>
       </c>
       <c r="J39" t="n">
         <v>1</v>
@@ -1916,34 +1987,34 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'HyperSQL'})</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>frozenset({'MS Access'})</t>
+          <t>frozenset({'SAP Adaptive Server'})</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.299492385786802</v>
+        <v>0.1384615384615385</v>
       </c>
       <c r="D40" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="E40" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="F40" t="n">
-        <v>0.1016949152542373</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="G40" t="n">
-        <v>3.338983050847458</v>
+        <v>4.814814814814814</v>
       </c>
       <c r="H40" t="n">
-        <v>0.02133525728568116</v>
+        <v>0.02437869822485207</v>
       </c>
       <c r="I40" t="n">
-        <v>1.079302748778852</v>
+        <v>1.226373626373626</v>
       </c>
       <c r="J40" t="n">
         <v>1</v>
@@ -1955,34 +2026,34 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'SAP SQL Anywhere'})</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>frozenset({'IBM DB2'})</t>
+          <t>frozenset({'HyperSQL'})</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.299492385786802</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="D41" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.1384615384615385</v>
       </c>
       <c r="E41" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="F41" t="n">
-        <v>0.1525423728813559</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G41" t="n">
-        <v>3.338983050847457</v>
+        <v>4.814814814814814</v>
       </c>
       <c r="H41" t="n">
-        <v>0.03200288592852173</v>
+        <v>0.02437869822485207</v>
       </c>
       <c r="I41" t="n">
-        <v>1.126091370558376</v>
+        <v>2.584615384615384</v>
       </c>
       <c r="J41" t="n">
         <v>1</v>
@@ -1994,7 +2065,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'MS Access'})</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2003,25 +2074,25 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.182741116751269</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="D42" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.1743589743589744</v>
       </c>
       <c r="E42" t="n">
-        <v>0.09137055837563451</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F42" t="n">
-        <v>0.5</v>
+        <v>0.8333333333333333</v>
       </c>
       <c r="G42" t="n">
-        <v>3.17741935483871</v>
+        <v>4.779411764705882</v>
       </c>
       <c r="H42" t="n">
-        <v>0.06261434203406427</v>
+        <v>0.02027613412228797</v>
       </c>
       <c r="I42" t="n">
-        <v>1.685279187817259</v>
+        <v>4.953846153846151</v>
       </c>
       <c r="J42" t="n">
         <v>1</v>
@@ -2038,29 +2109,29 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'MS Access'})</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.1743589743589744</v>
       </c>
       <c r="D43" t="n">
-        <v>0.182741116751269</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="E43" t="n">
-        <v>0.09137055837563451</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F43" t="n">
-        <v>0.5806451612903225</v>
+        <v>0.1470588235294118</v>
       </c>
       <c r="G43" t="n">
-        <v>3.17741935483871</v>
+        <v>4.779411764705882</v>
       </c>
       <c r="H43" t="n">
-        <v>0.06261434203406427</v>
+        <v>0.02027613412228797</v>
       </c>
       <c r="I43" t="n">
-        <v>1.948848106208512</v>
+        <v>1.136339522546419</v>
       </c>
       <c r="J43" t="n">
         <v>1</v>
@@ -2072,34 +2143,34 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>frozenset({'SQLite'})</t>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.182741116751269</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="D44" t="n">
-        <v>0.08121827411167512</v>
+        <v>0.1948717948717949</v>
       </c>
       <c r="E44" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.05128205128205128</v>
       </c>
       <c r="F44" t="n">
-        <v>0.25</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="G44" t="n">
-        <v>3.078125</v>
+        <v>4.665071770334928</v>
       </c>
       <c r="H44" t="n">
-        <v>0.03084336107603906</v>
+        <v>0.04028928336620644</v>
       </c>
       <c r="I44" t="n">
-        <v>1.225042301184433</v>
+        <v>8.856410256410253</v>
       </c>
       <c r="J44" t="n">
         <v>1</v>
@@ -2111,34 +2182,34 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>frozenset({'SQLite'})</t>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.08121827411167512</v>
+        <v>0.1948717948717949</v>
       </c>
       <c r="D45" t="n">
-        <v>0.182741116751269</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="E45" t="n">
-        <v>0.04568527918781726</v>
+        <v>0.05128205128205128</v>
       </c>
       <c r="F45" t="n">
-        <v>0.5625</v>
+        <v>0.2631578947368421</v>
       </c>
       <c r="G45" t="n">
-        <v>3.078125</v>
+        <v>4.665071770334928</v>
       </c>
       <c r="H45" t="n">
-        <v>0.03084336107603906</v>
+        <v>0.04028928336620644</v>
       </c>
       <c r="I45" t="n">
-        <v>1.868020304568528</v>
+        <v>1.28058608058608</v>
       </c>
       <c r="J45" t="n">
         <v>1</v>
@@ -2150,34 +2221,34 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'MS SQL Server_Microsoft Azure SQL Database'})</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.1948717948717949</v>
       </c>
       <c r="D46" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.05128205128205128</v>
       </c>
       <c r="E46" t="n">
-        <v>0.06091370558375635</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="F46" t="n">
-        <v>0.48</v>
+        <v>0.2368421052631579</v>
       </c>
       <c r="G46" t="n">
-        <v>3.050322580645162</v>
+        <v>4.61842105263158</v>
       </c>
       <c r="H46" t="n">
-        <v>0.04094411090211034</v>
+        <v>0.03616042077580539</v>
       </c>
       <c r="I46" t="n">
-        <v>1.620460757516595</v>
+        <v>1.24314765694076</v>
       </c>
       <c r="J46" t="n">
         <v>1</v>
@@ -2189,34 +2260,34 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'MS SQL Server_Microsoft Azure SQL Database'})</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.05128205128205128</v>
       </c>
       <c r="D47" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.1948717948717949</v>
       </c>
       <c r="E47" t="n">
-        <v>0.06091370558375635</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="F47" t="n">
-        <v>0.3870967741935484</v>
+        <v>0.9000000000000001</v>
       </c>
       <c r="G47" t="n">
-        <v>3.050322580645161</v>
+        <v>4.61842105263158</v>
       </c>
       <c r="H47" t="n">
-        <v>0.04094411090211034</v>
+        <v>0.03616042077580539</v>
       </c>
       <c r="I47" t="n">
-        <v>1.424525781458723</v>
+        <v>8.051282051282062</v>
       </c>
       <c r="J47" t="n">
         <v>1</v>
@@ -2228,34 +2299,34 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'SAP SQL Anywhere'})</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>frozenset({'MS SQL Server'})</t>
+          <t>frozenset({'H2'})</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.299492385786802</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="D48" t="n">
-        <v>0.04060913705583756</v>
+        <v>0.1743589743589744</v>
       </c>
       <c r="E48" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.03589743589743589</v>
       </c>
       <c r="F48" t="n">
-        <v>0.1186440677966102</v>
+        <v>0.7777777777777777</v>
       </c>
       <c r="G48" t="n">
-        <v>2.921610169491526</v>
+        <v>4.460784313725489</v>
       </c>
       <c r="H48" t="n">
-        <v>0.02337086758226185</v>
+        <v>0.02785009861932939</v>
       </c>
       <c r="I48" t="n">
-        <v>1.088539632955877</v>
+        <v>3.715384615384614</v>
       </c>
       <c r="J48" t="n">
         <v>1</v>
@@ -2267,34 +2338,34 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>frozenset({'MS SQL Server'})</t>
+          <t>frozenset({'H2'})</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'SAP SQL Anywhere'})</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.04060913705583756</v>
+        <v>0.1743589743589744</v>
       </c>
       <c r="D49" t="n">
-        <v>0.299492385786802</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="E49" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.03589743589743589</v>
       </c>
       <c r="F49" t="n">
-        <v>0.8750000000000001</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="G49" t="n">
-        <v>2.921610169491526</v>
+        <v>4.460784313725489</v>
       </c>
       <c r="H49" t="n">
-        <v>0.02337086758226185</v>
+        <v>0.02785009861932939</v>
       </c>
       <c r="I49" t="n">
-        <v>5.604060913705589</v>
+        <v>1.201139601139601</v>
       </c>
       <c r="J49" t="n">
         <v>1</v>
@@ -2306,34 +2377,34 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'H2'})</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'SAP Adaptive Server'})</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.1743589743589744</v>
       </c>
       <c r="D50" t="n">
-        <v>0.299492385786802</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="E50" t="n">
-        <v>0.1015228426395939</v>
+        <v>0.03589743589743589</v>
       </c>
       <c r="F50" t="n">
-        <v>0.8</v>
+        <v>0.2058823529411765</v>
       </c>
       <c r="G50" t="n">
-        <v>2.671186440677966</v>
+        <v>4.460784313725489</v>
       </c>
       <c r="H50" t="n">
-        <v>0.06351619469710634</v>
+        <v>0.02785009861932939</v>
       </c>
       <c r="I50" t="n">
-        <v>3.502538071065991</v>
+        <v>1.201139601139601</v>
       </c>
       <c r="J50" t="n">
         <v>1</v>
@@ -2345,34 +2416,34 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'SAP Adaptive Server'})</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'H2'})</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.299492385786802</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="D51" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.1743589743589744</v>
       </c>
       <c r="E51" t="n">
-        <v>0.1015228426395939</v>
+        <v>0.03589743589743589</v>
       </c>
       <c r="F51" t="n">
-        <v>0.3389830508474576</v>
+        <v>0.7777777777777777</v>
       </c>
       <c r="G51" t="n">
-        <v>2.671186440677966</v>
+        <v>4.460784313725489</v>
       </c>
       <c r="H51" t="n">
-        <v>0.06351619469710634</v>
+        <v>0.02785009861932939</v>
       </c>
       <c r="I51" t="n">
-        <v>1.320838214239229</v>
+        <v>3.715384615384614</v>
       </c>
       <c r="J51" t="n">
         <v>1</v>
@@ -2384,34 +2455,34 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>frozenset({'MongoDB'})</t>
+          <t>frozenset({'MS Access'})</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.299492385786802</v>
+        <v>0.1948717948717949</v>
       </c>
       <c r="D52" t="n">
-        <v>0.04060913705583756</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="E52" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F52" t="n">
-        <v>0.1016949152542373</v>
+        <v>0.131578947368421</v>
       </c>
       <c r="G52" t="n">
-        <v>2.504237288135593</v>
+        <v>4.276315789473684</v>
       </c>
       <c r="H52" t="n">
-        <v>0.01829472545028215</v>
+        <v>0.01964497041420118</v>
       </c>
       <c r="I52" t="n">
-        <v>1.0680011493152</v>
+        <v>1.116083916083916</v>
       </c>
       <c r="J52" t="n">
         <v>1</v>
@@ -2423,34 +2494,34 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>frozenset({'MongoDB'})</t>
+          <t>frozenset({'MS Access'})</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.04060913705583756</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="D53" t="n">
-        <v>0.299492385786802</v>
+        <v>0.1948717948717949</v>
       </c>
       <c r="E53" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F53" t="n">
-        <v>0.7500000000000001</v>
+        <v>0.8333333333333333</v>
       </c>
       <c r="G53" t="n">
-        <v>2.504237288135593</v>
+        <v>4.276315789473684</v>
       </c>
       <c r="H53" t="n">
-        <v>0.01829472545028215</v>
+        <v>0.01964497041420118</v>
       </c>
       <c r="I53" t="n">
-        <v>2.802030456852793</v>
+        <v>4.830769230769229</v>
       </c>
       <c r="J53" t="n">
         <v>1</v>
@@ -2462,34 +2533,34 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'H2'})</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.299492385786802</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="D54" t="n">
-        <v>0.182741116751269</v>
+        <v>0.1743589743589744</v>
       </c>
       <c r="E54" t="n">
-        <v>0.1370558375634518</v>
+        <v>0.04102564102564103</v>
       </c>
       <c r="F54" t="n">
-        <v>0.4576271186440677</v>
+        <v>0.7272727272727273</v>
       </c>
       <c r="G54" t="n">
-        <v>2.504237288135593</v>
+        <v>4.171122994652407</v>
       </c>
       <c r="H54" t="n">
-        <v>0.08232626452626968</v>
+        <v>0.03119000657462196</v>
       </c>
       <c r="I54" t="n">
-        <v>1.506821065989847</v>
+        <v>3.027350427350427</v>
       </c>
       <c r="J54" t="n">
         <v>1</v>
@@ -2501,34 +2572,34 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'H2'})</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0.182741116751269</v>
+        <v>0.1743589743589744</v>
       </c>
       <c r="D55" t="n">
-        <v>0.299492385786802</v>
+        <v>0.05641025641025641</v>
       </c>
       <c r="E55" t="n">
-        <v>0.1370558375634518</v>
+        <v>0.04102564102564103</v>
       </c>
       <c r="F55" t="n">
-        <v>0.75</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="G55" t="n">
-        <v>2.504237288135593</v>
+        <v>4.171122994652407</v>
       </c>
       <c r="H55" t="n">
-        <v>0.08232626452626968</v>
+        <v>0.03119000657462196</v>
       </c>
       <c r="I55" t="n">
-        <v>2.802030456852792</v>
+        <v>1.233925049309665</v>
       </c>
       <c r="J55" t="n">
         <v>1</v>
@@ -2540,34 +2611,34 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>frozenset({'SQLite'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.08121827411167512</v>
+        <v>0.1435897435897436</v>
       </c>
       <c r="D56" t="n">
-        <v>0.299492385786802</v>
+        <v>0.1948717948717949</v>
       </c>
       <c r="E56" t="n">
-        <v>0.05583756345177665</v>
+        <v>0.1128205128205128</v>
       </c>
       <c r="F56" t="n">
-        <v>0.6875000000000001</v>
+        <v>0.7857142857142858</v>
       </c>
       <c r="G56" t="n">
-        <v>2.295550847457628</v>
+        <v>4.031954887218046</v>
       </c>
       <c r="H56" t="n">
-        <v>0.03151330876858461</v>
+        <v>0.08483892176199868</v>
       </c>
       <c r="I56" t="n">
-        <v>2.241624365482234</v>
+        <v>3.757264957264959</v>
       </c>
       <c r="J56" t="n">
         <v>1</v>
@@ -2579,34 +2650,34 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>frozenset({'SQLite'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.299492385786802</v>
+        <v>0.1948717948717949</v>
       </c>
       <c r="D57" t="n">
-        <v>0.08121827411167512</v>
+        <v>0.1435897435897436</v>
       </c>
       <c r="E57" t="n">
-        <v>0.05583756345177665</v>
+        <v>0.1128205128205128</v>
       </c>
       <c r="F57" t="n">
-        <v>0.1864406779661017</v>
+        <v>0.5789473684210527</v>
       </c>
       <c r="G57" t="n">
-        <v>2.295550847457627</v>
+        <v>4.031954887218046</v>
       </c>
       <c r="H57" t="n">
-        <v>0.03151330876858461</v>
+        <v>0.08483892176199868</v>
       </c>
       <c r="I57" t="n">
-        <v>1.129335871404399</v>
+        <v>2.033974358974359</v>
       </c>
       <c r="J57" t="n">
         <v>1</v>
@@ -2618,34 +2689,34 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'SAP Adaptive Server'})</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.1948717948717949</v>
       </c>
       <c r="D58" t="n">
-        <v>0.299492385786802</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="E58" t="n">
-        <v>0.09644670050761421</v>
+        <v>0.03589743589743589</v>
       </c>
       <c r="F58" t="n">
-        <v>0.6129032258064516</v>
+        <v>0.1842105263157895</v>
       </c>
       <c r="G58" t="n">
-        <v>2.046473482777474</v>
+        <v>3.991228070175438</v>
       </c>
       <c r="H58" t="n">
-        <v>0.04931845705892963</v>
+        <v>0.02690335305719921</v>
       </c>
       <c r="I58" t="n">
-        <v>1.809644670050761</v>
+        <v>1.169230769230769</v>
       </c>
       <c r="J58" t="n">
         <v>1</v>
@@ -2657,34 +2728,34 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'SAP SQL Anywhere'})</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.299492385786802</v>
+        <v>0.1948717948717949</v>
       </c>
       <c r="D59" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="E59" t="n">
-        <v>0.09644670050761421</v>
+        <v>0.03589743589743589</v>
       </c>
       <c r="F59" t="n">
-        <v>0.3220338983050847</v>
+        <v>0.1842105263157895</v>
       </c>
       <c r="G59" t="n">
-        <v>2.046473482777474</v>
+        <v>3.991228070175438</v>
       </c>
       <c r="H59" t="n">
-        <v>0.04931845705892963</v>
+        <v>0.02690335305719921</v>
       </c>
       <c r="I59" t="n">
-        <v>1.242893401015228</v>
+        <v>1.169230769230769</v>
       </c>
       <c r="J59" t="n">
         <v>1</v>
@@ -2696,34 +2767,34 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'SAP SQL Anywhere'})</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>frozenset({'Ehcache'})</t>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="D60" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.1948717948717949</v>
       </c>
       <c r="E60" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.03589743589743589</v>
       </c>
       <c r="F60" t="n">
-        <v>0.24</v>
+        <v>0.7777777777777777</v>
       </c>
       <c r="G60" t="n">
-        <v>1.8912</v>
+        <v>3.991228070175438</v>
       </c>
       <c r="H60" t="n">
-        <v>0.01435234095184107</v>
+        <v>0.02690335305719921</v>
       </c>
       <c r="I60" t="n">
-        <v>1.148811114079615</v>
+        <v>3.623076923076922</v>
       </c>
       <c r="J60" t="n">
         <v>1</v>
@@ -2735,34 +2806,34 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>frozenset({'Ehcache'})</t>
+          <t>frozenset({'SAP Adaptive Server'})</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="D61" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.1948717948717949</v>
       </c>
       <c r="E61" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.03589743589743589</v>
       </c>
       <c r="F61" t="n">
-        <v>0.24</v>
+        <v>0.7777777777777777</v>
       </c>
       <c r="G61" t="n">
-        <v>1.8912</v>
+        <v>3.991228070175438</v>
       </c>
       <c r="H61" t="n">
-        <v>0.01435234095184107</v>
+        <v>0.02690335305719921</v>
       </c>
       <c r="I61" t="n">
-        <v>1.148811114079615</v>
+        <v>3.623076923076922</v>
       </c>
       <c r="J61" t="n">
         <v>1</v>
@@ -2774,34 +2845,34 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'HyperSQL'})</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>frozenset({'Ehcache'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.182741116751269</v>
+        <v>0.1384615384615385</v>
       </c>
       <c r="D62" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.1435897435897436</v>
       </c>
       <c r="E62" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.07179487179487179</v>
       </c>
       <c r="F62" t="n">
-        <v>0.1944444444444445</v>
+        <v>0.5185185185185185</v>
       </c>
       <c r="G62" t="n">
-        <v>1.532222222222223</v>
+        <v>3.611111111111111</v>
       </c>
       <c r="H62" t="n">
-        <v>0.01234249787420444</v>
+        <v>0.05191321499013806</v>
       </c>
       <c r="I62" t="n">
-        <v>1.083843864869596</v>
+        <v>1.778698224852071</v>
       </c>
       <c r="J62" t="n">
         <v>1</v>
@@ -2813,34 +2884,34 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>frozenset({'Ehcache'})</t>
+          <t>frozenset({'HyperSQL'})</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>frozenset({'PostgreSQL'})</t>
+          <t>frozenset({'MS SQL Server_Microsoft Azure SQL Database'})</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.1384615384615385</v>
       </c>
       <c r="D63" t="n">
-        <v>0.182741116751269</v>
+        <v>0.05128205128205128</v>
       </c>
       <c r="E63" t="n">
-        <v>0.03553299492385787</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F63" t="n">
-        <v>0.28</v>
+        <v>0.1851851851851852</v>
       </c>
       <c r="G63" t="n">
-        <v>1.532222222222222</v>
+        <v>3.611111111111111</v>
       </c>
       <c r="H63" t="n">
-        <v>0.01234249787420444</v>
+        <v>0.01854043392504931</v>
       </c>
       <c r="I63" t="n">
-        <v>1.135081782289904</v>
+        <v>1.164335664335664</v>
       </c>
       <c r="J63" t="n">
         <v>1</v>
@@ -2852,34 +2923,34 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>frozenset({'Ehcache'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'HyperSQL'})</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.1435897435897436</v>
       </c>
       <c r="D64" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.1384615384615385</v>
       </c>
       <c r="E64" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.07179487179487179</v>
       </c>
       <c r="F64" t="n">
-        <v>0.24</v>
+        <v>0.5</v>
       </c>
       <c r="G64" t="n">
-        <v>1.525161290322581</v>
+        <v>3.611111111111111</v>
       </c>
       <c r="H64" t="n">
-        <v>0.01048725811023217</v>
+        <v>0.05191321499013806</v>
       </c>
       <c r="I64" t="n">
-        <v>1.108736307774512</v>
+        <v>1.723076923076923</v>
       </c>
       <c r="J64" t="n">
         <v>1</v>
@@ -2891,34 +2962,34 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'MS SQL Server_Microsoft Azure SQL Database'})</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>frozenset({'Ehcache'})</t>
+          <t>frozenset({'HyperSQL'})</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.1573604060913706</v>
+        <v>0.05128205128205128</v>
       </c>
       <c r="D65" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.1384615384615385</v>
       </c>
       <c r="E65" t="n">
-        <v>0.03045685279187817</v>
+        <v>0.02564102564102564</v>
       </c>
       <c r="F65" t="n">
-        <v>0.1935483870967742</v>
+        <v>0.5</v>
       </c>
       <c r="G65" t="n">
-        <v>1.525161290322581</v>
+        <v>3.611111111111111</v>
       </c>
       <c r="H65" t="n">
-        <v>0.01048725811023217</v>
+        <v>0.01854043392504931</v>
       </c>
       <c r="I65" t="n">
-        <v>1.08263959390863</v>
+        <v>1.723076923076923</v>
       </c>
       <c r="J65" t="n">
         <v>1</v>
@@ -2930,34 +3001,34 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'MS SQL Server_Microsoft Azure SQL Database'})</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>frozenset({'Ehcache'})</t>
+          <t>frozenset({'H2'})</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0.299492385786802</v>
+        <v>0.05128205128205128</v>
       </c>
       <c r="D66" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.1743589743589744</v>
       </c>
       <c r="E66" t="n">
-        <v>0.05076142131979695</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="F66" t="n">
-        <v>0.1694915254237288</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="G66" t="n">
-        <v>1.335593220338983</v>
+        <v>3.441176470588236</v>
       </c>
       <c r="H66" t="n">
-        <v>0.01275477337730939</v>
+        <v>0.02182774490466798</v>
       </c>
       <c r="I66" t="n">
-        <v>1.051279395006734</v>
+        <v>2.064102564102564</v>
       </c>
       <c r="J66" t="n">
         <v>1</v>
@@ -2969,43 +3040,1927 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>frozenset({'Ehcache'})</t>
+          <t>frozenset({'H2'})</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'MS SQL Server_Microsoft Azure SQL Database'})</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0.1269035532994924</v>
+        <v>0.1743589743589744</v>
       </c>
       <c r="D67" t="n">
-        <v>0.299492385786802</v>
+        <v>0.05128205128205128</v>
       </c>
       <c r="E67" t="n">
-        <v>0.05076142131979695</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="F67" t="n">
+        <v>0.1764705882352941</v>
+      </c>
+      <c r="G67" t="n">
+        <v>3.441176470588236</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0.02182774490466798</v>
+      </c>
+      <c r="I67" t="n">
+        <v>1.152014652014652</v>
+      </c>
+      <c r="J67" t="n">
+        <v>1</v>
+      </c>
+      <c r="K67" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>frozenset({'SQLite'})</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>frozenset({'H2'})</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>0.08717948717948718</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.1743589743589744</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.05128205128205128</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.5882352941176471</v>
+      </c>
+      <c r="G68" t="n">
+        <v>3.373702422145329</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0.03608152531229454</v>
+      </c>
+      <c r="I68" t="n">
+        <v>2.005128205128205</v>
+      </c>
+      <c r="J68" t="n">
+        <v>1</v>
+      </c>
+      <c r="K68" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>frozenset({'H2'})</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>frozenset({'SQLite'})</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>0.1743589743589744</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.08717948717948718</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.05128205128205128</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.2941176470588235</v>
+      </c>
+      <c r="G69" t="n">
+        <v>3.373702422145329</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0.03608152531229454</v>
+      </c>
+      <c r="I69" t="n">
+        <v>1.293162393162393</v>
+      </c>
+      <c r="J69" t="n">
+        <v>1</v>
+      </c>
+      <c r="K69" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>frozenset({'Oracle'})</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>frozenset({'SQLite'})</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>0.1435897435897436</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.08717948717948718</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.04102564102564103</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.2857142857142858</v>
+      </c>
+      <c r="G70" t="n">
+        <v>3.277310924369749</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0.02850756081525312</v>
+      </c>
+      <c r="I70" t="n">
+        <v>1.277948717948718</v>
+      </c>
+      <c r="J70" t="n">
+        <v>1</v>
+      </c>
+      <c r="K70" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>frozenset({'SQLite'})</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>frozenset({'Oracle'})</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>0.08717948717948718</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.1435897435897436</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.04102564102564103</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.4705882352941177</v>
+      </c>
+      <c r="G71" t="n">
+        <v>3.277310924369749</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0.02850756081525312</v>
+      </c>
+      <c r="I71" t="n">
+        <v>1.617663817663818</v>
+      </c>
+      <c r="J71" t="n">
+        <v>1</v>
+      </c>
+      <c r="K71" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>frozenset({'Oracle'})</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>frozenset({'H2'})</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>0.1435897435897436</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.1743589743589744</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.07692307692307693</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.5357142857142858</v>
+      </c>
+      <c r="G72" t="n">
+        <v>3.072478991596639</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0.05188691650230112</v>
+      </c>
+      <c r="I72" t="n">
+        <v>1.778303747534517</v>
+      </c>
+      <c r="J72" t="n">
+        <v>1</v>
+      </c>
+      <c r="K72" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>frozenset({'H2'})</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>frozenset({'Oracle'})</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>0.1743589743589744</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.1435897435897436</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.07692307692307693</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.4411764705882353</v>
+      </c>
+      <c r="G73" t="n">
+        <v>3.072478991596639</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0.05188691650230112</v>
+      </c>
+      <c r="I73" t="n">
+        <v>1.532523616734143</v>
+      </c>
+      <c r="J73" t="n">
+        <v>1</v>
+      </c>
+      <c r="K73" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>frozenset({'HyperSQL'})</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>0.1948717948717949</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.1384615384615385</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.08205128205128205</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.4210526315789473</v>
+      </c>
+      <c r="G74" t="n">
+        <v>3.04093567251462</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0.05506903353057199</v>
+      </c>
+      <c r="I74" t="n">
+        <v>1.488111888111888</v>
+      </c>
+      <c r="J74" t="n">
+        <v>1</v>
+      </c>
+      <c r="K74" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>frozenset({'HyperSQL'})</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>0.1384615384615385</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.1948717948717949</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.08205128205128205</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.5925925925925926</v>
+      </c>
+      <c r="G75" t="n">
+        <v>3.04093567251462</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0.05506903353057199</v>
+      </c>
+      <c r="I75" t="n">
+        <v>1.976223776223776</v>
+      </c>
+      <c r="J75" t="n">
+        <v>1</v>
+      </c>
+      <c r="K75" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>frozenset({'SQLite'})</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>0.08717948717948718</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.1948717948717949</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.05128205128205128</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.5882352941176471</v>
+      </c>
+      <c r="G76" t="n">
+        <v>3.018575851393189</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0.03429322813938199</v>
+      </c>
+      <c r="I76" t="n">
+        <v>1.955311355311355</v>
+      </c>
+      <c r="J76" t="n">
+        <v>1</v>
+      </c>
+      <c r="K76" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>frozenset({'H2'})</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>0.1743589743589744</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.1948717948717949</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.1025641025641026</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.5882352941176471</v>
+      </c>
+      <c r="G77" t="n">
+        <v>3.018575851393189</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0.06858645627876397</v>
+      </c>
+      <c r="I77" t="n">
+        <v>1.955311355311355</v>
+      </c>
+      <c r="J77" t="n">
+        <v>1</v>
+      </c>
+      <c r="K77" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>frozenset({'SQLite'})</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>0.1948717948717949</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.08717948717948718</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.05128205128205128</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.2631578947368421</v>
+      </c>
+      <c r="G78" t="n">
+        <v>3.018575851393189</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0.03429322813938199</v>
+      </c>
+      <c r="I78" t="n">
+        <v>1.238827838827839</v>
+      </c>
+      <c r="J78" t="n">
+        <v>1</v>
+      </c>
+      <c r="K78" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>frozenset({'H2'})</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>0.1948717948717949</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.1743589743589744</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.1025641025641026</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.5263157894736842</v>
+      </c>
+      <c r="G79" t="n">
+        <v>3.018575851393189</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0.06858645627876397</v>
+      </c>
+      <c r="I79" t="n">
+        <v>1.743019943019943</v>
+      </c>
+      <c r="J79" t="n">
+        <v>1</v>
+      </c>
+      <c r="K79" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>frozenset({'MS SQL Server_Microsoft Azure SQL Database'})</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.05128205128205128</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.05128205128205128</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.1538461538461539</v>
+      </c>
+      <c r="G80" t="n">
+        <v>3</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0.03418803418803419</v>
+      </c>
+      <c r="I80" t="n">
+        <v>1.121212121212121</v>
+      </c>
+      <c r="J80" t="n">
+        <v>1</v>
+      </c>
+      <c r="K80" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>frozenset({'SAP SQL Anywhere'})</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>0.04615384615384616</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.04615384615384616</v>
+      </c>
+      <c r="F81" t="n">
+        <v>1</v>
+      </c>
+      <c r="G81" t="n">
+        <v>3</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+      <c r="J81" t="n">
+        <v>1</v>
+      </c>
+      <c r="K81" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>frozenset({'MS Access'})</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="F82" t="n">
+        <v>1</v>
+      </c>
+      <c r="G82" t="n">
+        <v>3</v>
+      </c>
+      <c r="H82" t="n">
+        <v>0.02051282051282052</v>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+      <c r="J82" t="n">
+        <v>1</v>
+      </c>
+      <c r="K82" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>frozenset({'IBM DB2'})</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>0.05641025641025641</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0.05641025641025641</v>
+      </c>
+      <c r="F83" t="n">
+        <v>1</v>
+      </c>
+      <c r="G83" t="n">
+        <v>3</v>
+      </c>
+      <c r="H83" t="n">
+        <v>0.03760683760683761</v>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+      <c r="J83" t="n">
+        <v>1</v>
+      </c>
+      <c r="K83" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>frozenset({'SAP SQL Anywhere'})</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.04615384615384616</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0.04615384615384616</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0.1384615384615385</v>
+      </c>
+      <c r="G84" t="n">
+        <v>3</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="I84" t="n">
+        <v>1.107142857142857</v>
+      </c>
+      <c r="J84" t="n">
+        <v>1</v>
+      </c>
+      <c r="K84" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>frozenset({'IBM DB2'})</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0.05641025641025641</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0.05641025641025641</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0.1692307692307692</v>
+      </c>
+      <c r="G85" t="n">
+        <v>3</v>
+      </c>
+      <c r="H85" t="n">
+        <v>0.03760683760683761</v>
+      </c>
+      <c r="I85" t="n">
+        <v>1.135802469135803</v>
+      </c>
+      <c r="J85" t="n">
+        <v>1</v>
+      </c>
+      <c r="K85" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>frozenset({'MS Access'})</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0.09230769230769231</v>
+      </c>
+      <c r="G86" t="n">
+        <v>3</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0.02051282051282052</v>
+      </c>
+      <c r="I86" t="n">
+        <v>1.067796610169492</v>
+      </c>
+      <c r="J86" t="n">
+        <v>1</v>
+      </c>
+      <c r="K86" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>frozenset({'MS SQL Server_Microsoft Azure SQL Database'})</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>0.05128205128205128</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0.05128205128205128</v>
+      </c>
+      <c r="F87" t="n">
+        <v>1</v>
+      </c>
+      <c r="G87" t="n">
+        <v>3</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0.03418803418803419</v>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+      <c r="J87" t="n">
+        <v>1</v>
+      </c>
+      <c r="K87" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>frozenset({'HBase'})</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="F88" t="n">
+        <v>1</v>
+      </c>
+      <c r="G88" t="n">
+        <v>3</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0.02051282051282052</v>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+      <c r="J88" t="n">
+        <v>1</v>
+      </c>
+      <c r="K88" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>frozenset({'HBase'})</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0.09230769230769231</v>
+      </c>
+      <c r="G89" t="n">
+        <v>3</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0.02051282051282052</v>
+      </c>
+      <c r="I89" t="n">
+        <v>1.067796610169492</v>
+      </c>
+      <c r="J89" t="n">
+        <v>1</v>
+      </c>
+      <c r="K89" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>frozenset({'SAP Adaptive Server'})</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0.04615384615384616</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.04615384615384616</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0.1384615384615385</v>
+      </c>
+      <c r="G90" t="n">
+        <v>3</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="I90" t="n">
+        <v>1.107142857142857</v>
+      </c>
+      <c r="J90" t="n">
+        <v>1</v>
+      </c>
+      <c r="K90" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>frozenset({'SAP Adaptive Server'})</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>0.04615384615384616</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0.04615384615384616</v>
+      </c>
+      <c r="F91" t="n">
+        <v>1</v>
+      </c>
+      <c r="G91" t="n">
+        <v>3</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
+      </c>
+      <c r="J91" t="n">
+        <v>1</v>
+      </c>
+      <c r="K91" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>frozenset({'HyperSQL'})</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>frozenset({'SQLite'})</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>0.1384615384615385</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.08717948717948718</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0.03589743589743589</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0.2592592592592592</v>
+      </c>
+      <c r="G92" t="n">
+        <v>2.973856209150327</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0.02382642998027613</v>
+      </c>
+      <c r="I92" t="n">
+        <v>1.232307692307692</v>
+      </c>
+      <c r="J92" t="n">
+        <v>1</v>
+      </c>
+      <c r="K92" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>frozenset({'SQLite'})</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>frozenset({'HyperSQL'})</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>0.08717948717948718</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.1384615384615385</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0.03589743589743589</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0.4117647058823529</v>
+      </c>
+      <c r="G93" t="n">
+        <v>2.973856209150326</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0.02382642998027613</v>
+      </c>
+      <c r="I93" t="n">
+        <v>1.464615384615385</v>
+      </c>
+      <c r="J93" t="n">
+        <v>1</v>
+      </c>
+      <c r="K93" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>frozenset({'MongoDB'})</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>0.05641025641025641</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.1948717948717949</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="F94" t="n">
+        <v>0.5454545454545455</v>
+      </c>
+      <c r="G94" t="n">
+        <v>2.799043062200957</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0.01977646285338593</v>
+      </c>
+      <c r="I94" t="n">
+        <v>1.771282051282052</v>
+      </c>
+      <c r="J94" t="n">
+        <v>1</v>
+      </c>
+      <c r="K94" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>frozenset({'MongoDB'})</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>0.1948717948717949</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0.05641025641025641</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0.1578947368421053</v>
+      </c>
+      <c r="G95" t="n">
+        <v>2.799043062200957</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0.01977646285338593</v>
+      </c>
+      <c r="I95" t="n">
+        <v>1.120512820512821</v>
+      </c>
+      <c r="J95" t="n">
+        <v>1</v>
+      </c>
+      <c r="K95" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>frozenset({'Oracle'})</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>0.1435897435897436</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="F96" t="n">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="G96" t="n">
+        <v>2.785714285714286</v>
+      </c>
+      <c r="H96" t="n">
+        <v>0.08547008547008547</v>
+      </c>
+      <c r="I96" t="n">
+        <v>9.333333333333339</v>
+      </c>
+      <c r="J96" t="n">
+        <v>1</v>
+      </c>
+      <c r="K96" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>frozenset({'Oracle'})</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0.1435897435897436</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="F97" t="n">
         <v>0.4</v>
       </c>
-      <c r="G67" t="n">
-        <v>1.335593220338983</v>
-      </c>
-      <c r="H67" t="n">
-        <v>0.01275477337730939</v>
-      </c>
-      <c r="I67" t="n">
-        <v>1.16751269035533</v>
-      </c>
-      <c r="J67" t="n">
-        <v>1</v>
-      </c>
-      <c r="K67" t="n">
+      <c r="G97" t="n">
+        <v>2.785714285714286</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0.08547008547008547</v>
+      </c>
+      <c r="I97" t="n">
+        <v>1.427350427350428</v>
+      </c>
+      <c r="J97" t="n">
+        <v>1</v>
+      </c>
+      <c r="K97" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>frozenset({'MongoDB'})</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>frozenset({'H2'})</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>0.05641025641025641</v>
+      </c>
+      <c r="D98" t="n">
+        <v>0.1743589743589744</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0.02564102564102564</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0.4545454545454545</v>
+      </c>
+      <c r="G98" t="n">
+        <v>2.606951871657754</v>
+      </c>
+      <c r="H98" t="n">
+        <v>0.01580539119000657</v>
+      </c>
+      <c r="I98" t="n">
+        <v>1.513675213675214</v>
+      </c>
+      <c r="J98" t="n">
+        <v>1</v>
+      </c>
+      <c r="K98" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>frozenset({'H2'})</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>frozenset({'MongoDB'})</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>0.1743589743589744</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0.05641025641025641</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0.02564102564102564</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0.1470588235294118</v>
+      </c>
+      <c r="G99" t="n">
+        <v>2.606951871657754</v>
+      </c>
+      <c r="H99" t="n">
+        <v>0.01580539119000657</v>
+      </c>
+      <c r="I99" t="n">
+        <v>1.106277630415561</v>
+      </c>
+      <c r="J99" t="n">
+        <v>1</v>
+      </c>
+      <c r="K99" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>frozenset({'HyperSQL'})</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>frozenset({'H2'})</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>0.1384615384615385</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0.1743589743589744</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0.06153846153846154</v>
+      </c>
+      <c r="F100" t="n">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="G100" t="n">
+        <v>2.549019607843137</v>
+      </c>
+      <c r="H100" t="n">
+        <v>0.03739644970414201</v>
+      </c>
+      <c r="I100" t="n">
+        <v>1.486153846153846</v>
+      </c>
+      <c r="J100" t="n">
+        <v>1</v>
+      </c>
+      <c r="K100" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>frozenset({'H2'})</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>frozenset({'HyperSQL'})</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>0.1743589743589744</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0.1384615384615385</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0.06153846153846154</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0.3529411764705883</v>
+      </c>
+      <c r="G101" t="n">
+        <v>2.549019607843137</v>
+      </c>
+      <c r="H101" t="n">
+        <v>0.03739644970414201</v>
+      </c>
+      <c r="I101" t="n">
+        <v>1.331468531468532</v>
+      </c>
+      <c r="J101" t="n">
+        <v>1</v>
+      </c>
+      <c r="K101" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0.1948717948717949</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0.1641025641025641</v>
+      </c>
+      <c r="F102" t="n">
+        <v>0.4923076923076923</v>
+      </c>
+      <c r="G102" t="n">
+        <v>2.526315789473685</v>
+      </c>
+      <c r="H102" t="n">
+        <v>0.09914529914529915</v>
+      </c>
+      <c r="I102" t="n">
+        <v>1.585858585858586</v>
+      </c>
+      <c r="J102" t="n">
+        <v>1</v>
+      </c>
+      <c r="K102" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>frozenset({'PostgreSQL_ CockroachDB'})</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>0.1948717948717949</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0.1641025641025641</v>
+      </c>
+      <c r="F103" t="n">
+        <v>0.8421052631578947</v>
+      </c>
+      <c r="G103" t="n">
+        <v>2.526315789473684</v>
+      </c>
+      <c r="H103" t="n">
+        <v>0.09914529914529915</v>
+      </c>
+      <c r="I103" t="n">
+        <v>4.222222222222221</v>
+      </c>
+      <c r="J103" t="n">
+        <v>1</v>
+      </c>
+      <c r="K103" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>frozenset({'Informix'})</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="D104" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0.02564102564102564</v>
+      </c>
+      <c r="F104" t="n">
+        <v>0.8333333333333333</v>
+      </c>
+      <c r="G104" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H104" t="n">
+        <v>0.01538461538461538</v>
+      </c>
+      <c r="I104" t="n">
+        <v>3.999999999999999</v>
+      </c>
+      <c r="J104" t="n">
+        <v>1</v>
+      </c>
+      <c r="K104" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>frozenset({'Informix'})</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D105" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0.02564102564102564</v>
+      </c>
+      <c r="F105" t="n">
+        <v>0.07692307692307693</v>
+      </c>
+      <c r="G105" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H105" t="n">
+        <v>0.01538461538461538</v>
+      </c>
+      <c r="I105" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="J105" t="n">
+        <v>1</v>
+      </c>
+      <c r="K105" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>frozenset({'MongoDB'})</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>0.05641025641025641</v>
+      </c>
+      <c r="D106" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0.04102564102564103</v>
+      </c>
+      <c r="F106" t="n">
+        <v>0.7272727272727273</v>
+      </c>
+      <c r="G106" t="n">
+        <v>2.181818181818182</v>
+      </c>
+      <c r="H106" t="n">
+        <v>0.02222222222222222</v>
+      </c>
+      <c r="I106" t="n">
+        <v>2.444444444444445</v>
+      </c>
+      <c r="J106" t="n">
+        <v>1</v>
+      </c>
+      <c r="K106" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>frozenset({'MongoDB'})</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D107" t="n">
+        <v>0.05641025641025641</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0.04102564102564103</v>
+      </c>
+      <c r="F107" t="n">
+        <v>0.1230769230769231</v>
+      </c>
+      <c r="G107" t="n">
+        <v>2.181818181818182</v>
+      </c>
+      <c r="H107" t="n">
+        <v>0.02222222222222222</v>
+      </c>
+      <c r="I107" t="n">
+        <v>1.076023391812865</v>
+      </c>
+      <c r="J107" t="n">
+        <v>1</v>
+      </c>
+      <c r="K107" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>frozenset({'SQLite'})</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>0.08717948717948718</v>
+      </c>
+      <c r="D108" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0.06153846153846154</v>
+      </c>
+      <c r="F108" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="G108" t="n">
+        <v>2.11764705882353</v>
+      </c>
+      <c r="H108" t="n">
+        <v>0.03247863247863249</v>
+      </c>
+      <c r="I108" t="n">
+        <v>2.266666666666667</v>
+      </c>
+      <c r="J108" t="n">
+        <v>1</v>
+      </c>
+      <c r="K108" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>frozenset({'H2'})</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>0.1743589743589744</v>
+      </c>
+      <c r="D109" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0.1230769230769231</v>
+      </c>
+      <c r="F109" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="G109" t="n">
+        <v>2.11764705882353</v>
+      </c>
+      <c r="H109" t="n">
+        <v>0.06495726495726498</v>
+      </c>
+      <c r="I109" t="n">
+        <v>2.266666666666667</v>
+      </c>
+      <c r="J109" t="n">
+        <v>1</v>
+      </c>
+      <c r="K109" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>frozenset({'SQLite'})</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D110" t="n">
+        <v>0.08717948717948718</v>
+      </c>
+      <c r="E110" t="n">
+        <v>0.06153846153846154</v>
+      </c>
+      <c r="F110" t="n">
+        <v>0.1846153846153846</v>
+      </c>
+      <c r="G110" t="n">
+        <v>2.117647058823529</v>
+      </c>
+      <c r="H110" t="n">
+        <v>0.03247863247863249</v>
+      </c>
+      <c r="I110" t="n">
+        <v>1.119496855345912</v>
+      </c>
+      <c r="J110" t="n">
+        <v>1</v>
+      </c>
+      <c r="K110" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>frozenset({'H2'})</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D111" t="n">
+        <v>0.1743589743589744</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0.1230769230769231</v>
+      </c>
+      <c r="F111" t="n">
+        <v>0.3692307692307693</v>
+      </c>
+      <c r="G111" t="n">
+        <v>2.117647058823529</v>
+      </c>
+      <c r="H111" t="n">
+        <v>0.06495726495726498</v>
+      </c>
+      <c r="I111" t="n">
+        <v>1.308943089430894</v>
+      </c>
+      <c r="J111" t="n">
+        <v>1</v>
+      </c>
+      <c r="K111" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>frozenset({'HyperSQL'})</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>0.1384615384615385</v>
+      </c>
+      <c r="D112" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0.09230769230769231</v>
+      </c>
+      <c r="F112" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="G112" t="n">
+        <v>2</v>
+      </c>
+      <c r="H112" t="n">
+        <v>0.04615384615384616</v>
+      </c>
+      <c r="I112" t="n">
+        <v>2</v>
+      </c>
+      <c r="J112" t="n">
+        <v>1</v>
+      </c>
+      <c r="K112" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>frozenset({'HyperSQL'})</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D113" t="n">
+        <v>0.1384615384615385</v>
+      </c>
+      <c r="E113" t="n">
+        <v>0.09230769230769231</v>
+      </c>
+      <c r="F113" t="n">
+        <v>0.2769230769230769</v>
+      </c>
+      <c r="G113" t="n">
+        <v>2</v>
+      </c>
+      <c r="H113" t="n">
+        <v>0.04615384615384616</v>
+      </c>
+      <c r="I113" t="n">
+        <v>1.191489361702128</v>
+      </c>
+      <c r="J113" t="n">
+        <v>1</v>
+      </c>
+      <c r="K113" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>frozenset({'Redis'})</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E114" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="F114" t="n">
+        <v>0.4615384615384616</v>
+      </c>
+      <c r="G114" t="n">
+        <v>1.384615384615385</v>
+      </c>
+      <c r="H114" t="n">
+        <v>0.008547008547008551</v>
+      </c>
+      <c r="I114" t="n">
+        <v>1.238095238095238</v>
+      </c>
+      <c r="J114" t="n">
+        <v>1</v>
+      </c>
+      <c r="K114" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>frozenset({'MySQL_Maria DB'})</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>frozenset({'Redis'})</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="E115" t="n">
+        <v>0.03076923076923077</v>
+      </c>
+      <c r="F115" t="n">
+        <v>0.09230769230769231</v>
+      </c>
+      <c r="G115" t="n">
+        <v>1.384615384615385</v>
+      </c>
+      <c r="H115" t="n">
+        <v>0.008547008547008551</v>
+      </c>
+      <c r="I115" t="n">
+        <v>1.028248587570622</v>
+      </c>
+      <c r="J115" t="n">
+        <v>1</v>
+      </c>
+      <c r="K115" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New results RQ4 version1
</commit_message>
<xml_diff>
--- a/resources/historical_rulesv1.xlsx
+++ b/resources/historical_rulesv1.xlsx
@@ -493,25 +493,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>frozenset({'IBM DB2'})</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>frozenset({'MS SQL Server'})</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>frozenset({'IBM DB2'})</t>
-        </is>
-      </c>
       <c r="C2" t="n">
+        <v>0.04310344827586207</v>
+      </c>
+      <c r="D2" t="n">
         <v>0.03879310344827586</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.04310344827586207</v>
       </c>
       <c r="E2" t="n">
         <v>0.02155172413793104</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.5</v>
       </c>
       <c r="G2" t="n">
         <v>12.88888888888889</v>
@@ -520,7 +520,7 @@
         <v>0.01987960760998811</v>
       </c>
       <c r="I2" t="n">
-        <v>2.15301724137931</v>
+        <v>1.922413793103448</v>
       </c>
       <c r="J2" t="n">
         <v>1</v>
@@ -532,25 +532,25 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>frozenset({'MS SQL Server'})</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>frozenset({'MS SQL Server'})</t>
-        </is>
-      </c>
       <c r="C3" t="n">
+        <v>0.03879310344827586</v>
+      </c>
+      <c r="D3" t="n">
         <v>0.04310344827586207</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.03879310344827586</v>
       </c>
       <c r="E3" t="n">
         <v>0.02155172413793104</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="G3" t="n">
         <v>12.88888888888889</v>
@@ -559,7 +559,7 @@
         <v>0.01987960760998811</v>
       </c>
       <c r="I3" t="n">
-        <v>1.922413793103448</v>
+        <v>2.15301724137931</v>
       </c>
       <c r="J3" t="n">
         <v>1</v>
@@ -885,25 +885,25 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>frozenset({'MS SQL Server'})</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>frozenset({'Oracle'})</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>frozenset({'MS SQL Server'})</t>
-        </is>
-      </c>
       <c r="C12" t="n">
+        <v>0.03879310344827586</v>
+      </c>
+      <c r="D12" t="n">
         <v>0.08620689655172414</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.03879310344827586</v>
       </c>
       <c r="E12" t="n">
         <v>0.03017241379310345</v>
       </c>
       <c r="F12" t="n">
-        <v>0.35</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="G12" t="n">
         <v>9.022222222222222</v>
@@ -912,7 +912,7 @@
         <v>0.0268281807372176</v>
       </c>
       <c r="I12" t="n">
-        <v>1.478779840848806</v>
+        <v>4.112068965517241</v>
       </c>
       <c r="J12" t="n">
         <v>1</v>
@@ -924,25 +924,25 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>frozenset({'Oracle'})</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>frozenset({'MS SQL Server'})</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>frozenset({'Oracle'})</t>
-        </is>
-      </c>
       <c r="C13" t="n">
+        <v>0.08620689655172414</v>
+      </c>
+      <c r="D13" t="n">
         <v>0.03879310344827586</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.08620689655172414</v>
       </c>
       <c r="E13" t="n">
         <v>0.03017241379310345</v>
       </c>
       <c r="F13" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.35</v>
       </c>
       <c r="G13" t="n">
         <v>9.022222222222222</v>
@@ -951,7 +951,7 @@
         <v>0.0268281807372176</v>
       </c>
       <c r="I13" t="n">
-        <v>4.112068965517241</v>
+        <v>1.478779840848806</v>
       </c>
       <c r="J13" t="n">
         <v>1</v>
@@ -1041,25 +1041,25 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>frozenset({'IBM DB2'})</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>frozenset({'PostgreSQL'})</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>frozenset({'IBM DB2'})</t>
-        </is>
-      </c>
       <c r="C16" t="n">
+        <v>0.04310344827586207</v>
+      </c>
+      <c r="D16" t="n">
         <v>0.09913793103448276</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.04310344827586207</v>
       </c>
       <c r="E16" t="n">
         <v>0.03448275862068965</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3478260869565217</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="G16" t="n">
         <v>8.069565217391304</v>
@@ -1068,7 +1068,7 @@
         <v>0.03020957193816885</v>
       </c>
       <c r="I16" t="n">
-        <v>1.467241379310345</v>
+        <v>4.504310344827585</v>
       </c>
       <c r="J16" t="n">
         <v>1</v>
@@ -1080,25 +1080,25 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>frozenset({'PostgreSQL'})</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>frozenset({'PostgreSQL'})</t>
-        </is>
-      </c>
       <c r="C17" t="n">
+        <v>0.09913793103448276</v>
+      </c>
+      <c r="D17" t="n">
         <v>0.04310344827586207</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.09913793103448276</v>
       </c>
       <c r="E17" t="n">
         <v>0.03448275862068965</v>
       </c>
       <c r="F17" t="n">
-        <v>0.7999999999999999</v>
+        <v>0.3478260869565217</v>
       </c>
       <c r="G17" t="n">
         <v>8.069565217391304</v>
@@ -1107,7 +1107,7 @@
         <v>0.03020957193816885</v>
       </c>
       <c r="I17" t="n">
-        <v>4.504310344827585</v>
+        <v>1.467241379310345</v>
       </c>
       <c r="J17" t="n">
         <v>1</v>
@@ -1119,7 +1119,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>frozenset({'IBM DB2'})</t>
+          <t>frozenset({'Informix'})</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1128,13 +1128,13 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.02155172413793104</v>
       </c>
       <c r="D18" t="n">
         <v>0.1379310344827586</v>
       </c>
       <c r="E18" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.02155172413793104</v>
       </c>
       <c r="F18" t="n">
         <v>1</v>
@@ -1143,7 +1143,7 @@
         <v>7.25</v>
       </c>
       <c r="H18" t="n">
-        <v>0.03715814506539834</v>
+        <v>0.01857907253269917</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1160,7 +1160,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>frozenset({'Informix'})</t>
+          <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1169,13 +1169,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.04310344827586207</v>
       </c>
       <c r="D19" t="n">
         <v>0.1379310344827586</v>
       </c>
       <c r="E19" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.04310344827586207</v>
       </c>
       <c r="F19" t="n">
         <v>1</v>
@@ -1184,7 +1184,7 @@
         <v>7.25</v>
       </c>
       <c r="H19" t="n">
-        <v>0.01857907253269917</v>
+        <v>0.03715814506539834</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1981,36 +1981,34 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>frozenset({'MS SQL Server'})</t>
+          <t>frozenset({'H2'})</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.1163793103448276</v>
       </c>
       <c r="D40" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.04310344827586207</v>
       </c>
       <c r="E40" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.02155172413793104</v>
       </c>
       <c r="F40" t="n">
-        <v>1</v>
+        <v>0.1851851851851852</v>
       </c>
       <c r="G40" t="n">
         <v>4.296296296296297</v>
       </c>
       <c r="H40" t="n">
-        <v>0.02976367419738407</v>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>0.01653537455410226</v>
+      </c>
+      <c r="I40" t="n">
+        <v>1.174373040752351</v>
       </c>
       <c r="J40" t="n">
         <v>1</v>
@@ -2022,34 +2020,36 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>frozenset({'MS Access'})</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
           <t>frozenset({'MySQL'})</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>frozenset({'MS SQL Server'})</t>
-        </is>
-      </c>
       <c r="C41" t="n">
+        <v>0.03017241379310345</v>
+      </c>
+      <c r="D41" t="n">
         <v>0.2327586206896552</v>
       </c>
-      <c r="D41" t="n">
-        <v>0.03879310344827586</v>
-      </c>
       <c r="E41" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.03017241379310345</v>
       </c>
       <c r="F41" t="n">
-        <v>0.1666666666666667</v>
+        <v>1</v>
       </c>
       <c r="G41" t="n">
         <v>4.296296296296297</v>
       </c>
       <c r="H41" t="n">
-        <v>0.02976367419738407</v>
-      </c>
-      <c r="I41" t="n">
-        <v>1.153448275862069</v>
+        <v>0.02314952437574316</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
       <c r="J41" t="n">
         <v>1</v>
@@ -2061,25 +2061,25 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
+          <t>frozenset({'MySQL'})</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
           <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>frozenset({'MySQL'})</t>
-        </is>
-      </c>
       <c r="C42" t="n">
+        <v>0.2327586206896552</v>
+      </c>
+      <c r="D42" t="n">
         <v>0.04310344827586207</v>
-      </c>
-      <c r="D42" t="n">
-        <v>0.2327586206896552</v>
       </c>
       <c r="E42" t="n">
         <v>0.04310344827586207</v>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>0.1851851851851852</v>
       </c>
       <c r="G42" t="n">
         <v>4.296296296296297</v>
@@ -2087,10 +2087,8 @@
       <c r="H42" t="n">
         <v>0.03307074910820453</v>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="I42" t="n">
+        <v>1.174373040752351</v>
       </c>
       <c r="J42" t="n">
         <v>1</v>
@@ -2107,29 +2105,29 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>frozenset({'IBM DB2'})</t>
+          <t>frozenset({'MS Access'})</t>
         </is>
       </c>
       <c r="C43" t="n">
         <v>0.2327586206896552</v>
       </c>
       <c r="D43" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.03017241379310345</v>
       </c>
       <c r="E43" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.03017241379310345</v>
       </c>
       <c r="F43" t="n">
-        <v>0.1851851851851852</v>
+        <v>0.1296296296296297</v>
       </c>
       <c r="G43" t="n">
         <v>4.296296296296297</v>
       </c>
       <c r="H43" t="n">
-        <v>0.03307074910820453</v>
+        <v>0.02314952437574316</v>
       </c>
       <c r="I43" t="n">
-        <v>1.174373040752351</v>
+        <v>1.114269992663243</v>
       </c>
       <c r="J43" t="n">
         <v>1</v>
@@ -2141,7 +2139,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>frozenset({'MS Access'})</t>
+          <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2150,13 +2148,13 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.04310344827586207</v>
       </c>
       <c r="D44" t="n">
         <v>0.2327586206896552</v>
       </c>
       <c r="E44" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.04310344827586207</v>
       </c>
       <c r="F44" t="n">
         <v>1</v>
@@ -2165,7 +2163,7 @@
         <v>4.296296296296297</v>
       </c>
       <c r="H44" t="n">
-        <v>0.02314952437574316</v>
+        <v>0.03307074910820453</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
@@ -2182,34 +2180,36 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
+          <t>frozenset({'MS SQL Server'})</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
           <t>frozenset({'MySQL'})</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>frozenset({'MS Access'})</t>
-        </is>
-      </c>
       <c r="C45" t="n">
+        <v>0.03879310344827586</v>
+      </c>
+      <c r="D45" t="n">
         <v>0.2327586206896552</v>
       </c>
-      <c r="D45" t="n">
-        <v>0.03017241379310345</v>
-      </c>
       <c r="E45" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03879310344827586</v>
       </c>
       <c r="F45" t="n">
-        <v>0.1296296296296297</v>
+        <v>1</v>
       </c>
       <c r="G45" t="n">
         <v>4.296296296296297</v>
       </c>
       <c r="H45" t="n">
-        <v>0.02314952437574316</v>
-      </c>
-      <c r="I45" t="n">
-        <v>1.114269992663243</v>
+        <v>0.02976367419738407</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
       <c r="J45" t="n">
         <v>1</v>
@@ -2221,34 +2221,34 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>frozenset({'IBM DB2'})</t>
+          <t>frozenset({'MySQL'})</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'MS SQL Server'})</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.2327586206896552</v>
       </c>
       <c r="D46" t="n">
-        <v>0.1163793103448276</v>
+        <v>0.03879310344827586</v>
       </c>
       <c r="E46" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.03879310344827586</v>
       </c>
       <c r="F46" t="n">
-        <v>0.5</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="G46" t="n">
         <v>4.296296296296297</v>
       </c>
       <c r="H46" t="n">
-        <v>0.01653537455410226</v>
+        <v>0.02976367419738407</v>
       </c>
       <c r="I46" t="n">
-        <v>1.767241379310345</v>
+        <v>1.153448275862069</v>
       </c>
       <c r="J46" t="n">
         <v>1</v>
@@ -2260,25 +2260,25 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
+          <t>frozenset({'IBM DB2'})</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
           <t>frozenset({'H2'})</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>frozenset({'IBM DB2'})</t>
-        </is>
-      </c>
       <c r="C47" t="n">
+        <v>0.04310344827586207</v>
+      </c>
+      <c r="D47" t="n">
         <v>0.1163793103448276</v>
-      </c>
-      <c r="D47" t="n">
-        <v>0.04310344827586207</v>
       </c>
       <c r="E47" t="n">
         <v>0.02155172413793104</v>
       </c>
       <c r="F47" t="n">
-        <v>0.1851851851851852</v>
+        <v>0.5</v>
       </c>
       <c r="G47" t="n">
         <v>4.296296296296297</v>
@@ -2287,7 +2287,7 @@
         <v>0.01653537455410226</v>
       </c>
       <c r="I47" t="n">
-        <v>1.174373040752351</v>
+        <v>1.767241379310345</v>
       </c>
       <c r="J47" t="n">
         <v>1</v>
@@ -2455,25 +2455,25 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
+          <t>frozenset({'H2'})</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
           <t>frozenset({'PostgreSQL'})</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>frozenset({'H2'})</t>
-        </is>
-      </c>
       <c r="C52" t="n">
+        <v>0.1163793103448276</v>
+      </c>
+      <c r="D52" t="n">
         <v>0.09913793103448276</v>
-      </c>
-      <c r="D52" t="n">
-        <v>0.1163793103448276</v>
       </c>
       <c r="E52" t="n">
         <v>0.04310344827586207</v>
       </c>
       <c r="F52" t="n">
-        <v>0.4347826086956522</v>
+        <v>0.3703703703703704</v>
       </c>
       <c r="G52" t="n">
         <v>3.735909822866345</v>
@@ -2482,7 +2482,7 @@
         <v>0.03156584423305589</v>
       </c>
       <c r="I52" t="n">
-        <v>1.563328912466843</v>
+        <v>1.43078093306288</v>
       </c>
       <c r="J52" t="n">
         <v>1</v>
@@ -2494,25 +2494,25 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
+          <t>frozenset({'PostgreSQL'})</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
           <t>frozenset({'H2'})</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>frozenset({'PostgreSQL'})</t>
-        </is>
-      </c>
       <c r="C53" t="n">
+        <v>0.09913793103448276</v>
+      </c>
+      <c r="D53" t="n">
         <v>0.1163793103448276</v>
-      </c>
-      <c r="D53" t="n">
-        <v>0.09913793103448276</v>
       </c>
       <c r="E53" t="n">
         <v>0.04310344827586207</v>
       </c>
       <c r="F53" t="n">
-        <v>0.3703703703703704</v>
+        <v>0.4347826086956522</v>
       </c>
       <c r="G53" t="n">
         <v>3.735909822866345</v>
@@ -2521,7 +2521,7 @@
         <v>0.03156584423305589</v>
       </c>
       <c r="I53" t="n">
-        <v>1.43078093306288</v>
+        <v>1.563328912466843</v>
       </c>
       <c r="J53" t="n">
         <v>1</v>
@@ -2689,34 +2689,34 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>frozenset({'HyperSQL'})</t>
+          <t>frozenset({'MySQL'})</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.1163793103448276</v>
+        <v>0.08620689655172414</v>
       </c>
       <c r="D58" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.2327586206896552</v>
       </c>
       <c r="E58" t="n">
-        <v>0.05172413793103448</v>
+        <v>0.06465517241379311</v>
       </c>
       <c r="F58" t="n">
-        <v>0.4444444444444445</v>
+        <v>0.75</v>
       </c>
       <c r="G58" t="n">
         <v>3.222222222222222</v>
       </c>
       <c r="H58" t="n">
-        <v>0.0356718192627824</v>
+        <v>0.04458977407847801</v>
       </c>
       <c r="I58" t="n">
-        <v>1.551724137931034</v>
+        <v>3.068965517241379</v>
       </c>
       <c r="J58" t="n">
         <v>1</v>
@@ -2767,34 +2767,34 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'HyperSQL'})</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'H2'})</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.1379310344827586</v>
       </c>
       <c r="D60" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.1163793103448276</v>
       </c>
       <c r="E60" t="n">
-        <v>0.06465517241379311</v>
+        <v>0.05172413793103448</v>
       </c>
       <c r="F60" t="n">
-        <v>0.75</v>
+        <v>0.375</v>
       </c>
       <c r="G60" t="n">
         <v>3.222222222222222</v>
       </c>
       <c r="H60" t="n">
-        <v>0.04458977407847801</v>
+        <v>0.0356718192627824</v>
       </c>
       <c r="I60" t="n">
-        <v>3.068965517241379</v>
+        <v>1.413793103448276</v>
       </c>
       <c r="J60" t="n">
         <v>1</v>
@@ -2806,25 +2806,25 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
+          <t>frozenset({'H2'})</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
           <t>frozenset({'HyperSQL'})</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>frozenset({'H2'})</t>
-        </is>
-      </c>
       <c r="C61" t="n">
+        <v>0.1163793103448276</v>
+      </c>
+      <c r="D61" t="n">
         <v>0.1379310344827586</v>
-      </c>
-      <c r="D61" t="n">
-        <v>0.1163793103448276</v>
       </c>
       <c r="E61" t="n">
         <v>0.05172413793103448</v>
       </c>
       <c r="F61" t="n">
-        <v>0.375</v>
+        <v>0.4444444444444445</v>
       </c>
       <c r="G61" t="n">
         <v>3.222222222222222</v>
@@ -2833,7 +2833,7 @@
         <v>0.0356718192627824</v>
       </c>
       <c r="I61" t="n">
-        <v>1.413793103448276</v>
+        <v>1.551724137931034</v>
       </c>
       <c r="J61" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Update RQ3 table and start to update RQ4
</commit_message>
<xml_diff>
--- a/resources/historical_rulesv1.xlsx
+++ b/resources/historical_rulesv1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,10 +481,15 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>zhangs_metric</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>antecedent_len</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>consequente_len</t>
         </is>
@@ -502,30 +507,33 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="E2" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="F2" t="n">
         <v>0.5</v>
       </c>
       <c r="G2" t="n">
-        <v>12.88888888888889</v>
+        <v>12.94444444444444</v>
       </c>
       <c r="H2" t="n">
-        <v>0.01987960760998811</v>
+        <v>0.01980143307115622</v>
       </c>
       <c r="I2" t="n">
-        <v>1.922413793103448</v>
+        <v>1.92274678111588</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>0.9641255605381166</v>
       </c>
       <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -541,266 +549,287 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="D3" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="E3" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.5555555555555555</v>
       </c>
       <c r="G3" t="n">
-        <v>12.88888888888889</v>
+        <v>12.94444444444444</v>
       </c>
       <c r="H3" t="n">
-        <v>0.01987960760998811</v>
+        <v>0.01980143307115622</v>
       </c>
       <c r="I3" t="n">
-        <v>2.15301724137931</v>
+        <v>2.153433476394849</v>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>0.9598214285714287</v>
       </c>
       <c r="K3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>frozenset({'SQLite'})</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>frozenset({'MS SQL Server'})</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>frozenset({'SQLite'})</t>
-        </is>
-      </c>
       <c r="C4" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.05150214592274678</v>
       </c>
       <c r="D4" t="n">
-        <v>0.05172413793103448</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="E4" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="G4" t="n">
-        <v>10.74074074074074</v>
+        <v>10.78703703703704</v>
       </c>
       <c r="H4" t="n">
-        <v>0.01954518430439953</v>
+        <v>0.01946987419182523</v>
       </c>
       <c r="I4" t="n">
-        <v>2.133620689655173</v>
+        <v>1.648068669527897</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>0.9565610859728507</v>
       </c>
       <c r="K4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>frozenset({'MS SQL Server'})</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>frozenset({'SQLite'})</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>frozenset({'MS SQL Server'})</t>
-        </is>
-      </c>
       <c r="C5" t="n">
-        <v>0.05172413793103448</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="D5" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.05150214592274678</v>
       </c>
       <c r="E5" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.5555555555555555</v>
       </c>
       <c r="G5" t="n">
-        <v>10.74074074074074</v>
+        <v>10.78703703703703</v>
       </c>
       <c r="H5" t="n">
-        <v>0.01954518430439953</v>
+        <v>0.01946987419182523</v>
       </c>
       <c r="I5" t="n">
-        <v>1.647783251231527</v>
+        <v>2.134120171673819</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>0.9437500000000001</v>
       </c>
       <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>frozenset({'Oracle'})</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>frozenset({'Oracle'})</t>
-        </is>
-      </c>
       <c r="C6" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="D6" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="E6" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9</v>
+        <v>0.4500000000000001</v>
       </c>
       <c r="G6" t="n">
-        <v>10.44</v>
+        <v>10.485</v>
       </c>
       <c r="H6" t="n">
-        <v>0.03507728894173603</v>
+        <v>0.034942621893938</v>
       </c>
       <c r="I6" t="n">
-        <v>9.13793103448276</v>
+        <v>1.740148263753414</v>
       </c>
       <c r="J6" t="n">
-        <v>1</v>
+        <v>0.9895670318205528</v>
       </c>
       <c r="K6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>frozenset({'IBM DB2'})</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>frozenset({'Oracle'})</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>frozenset({'IBM DB2'})</t>
-        </is>
-      </c>
       <c r="C7" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="D7" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="E7" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="F7" t="n">
-        <v>0.45</v>
+        <v>0.9000000000000001</v>
       </c>
       <c r="G7" t="n">
-        <v>10.44</v>
+        <v>10.485</v>
       </c>
       <c r="H7" t="n">
-        <v>0.03507728894173603</v>
+        <v>0.034942621893938</v>
       </c>
       <c r="I7" t="n">
-        <v>1.739811912225705</v>
+        <v>9.141630901287567</v>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>0.9451918285999003</v>
       </c>
       <c r="K7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>frozenset({'PostgreSQL'})</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>frozenset({'Informix'})</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>frozenset({'PostgreSQL'})</t>
-        </is>
-      </c>
       <c r="C8" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="D8" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="E8" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>0.2173913043478261</v>
       </c>
       <c r="G8" t="n">
-        <v>10.08695652173913</v>
+        <v>10.1304347826087</v>
       </c>
       <c r="H8" t="n">
-        <v>0.01941513079667063</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>0.01934093462764096</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1.25035765379113</v>
       </c>
       <c r="J8" t="n">
         <v>1</v>
       </c>
       <c r="K8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>frozenset({'Informix'})</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>frozenset({'PostgreSQL'})</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>frozenset({'Informix'})</t>
-        </is>
-      </c>
       <c r="C9" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="D9" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="E9" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2173913043478261</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>10.08695652173913</v>
+        <v>10.1304347826087</v>
       </c>
       <c r="H9" t="n">
-        <v>0.01941513079667063</v>
-      </c>
-      <c r="I9" t="n">
-        <v>1.250239463601533</v>
+        <v>0.01934093462764096</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>0.9210526315789472</v>
       </c>
       <c r="K9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -816,30 +845,33 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="D10" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="E10" t="n">
-        <v>0.02586206896551724</v>
+        <v>0.02575107296137339</v>
       </c>
       <c r="F10" t="n">
         <v>0.3</v>
       </c>
       <c r="G10" t="n">
-        <v>9.942857142857141</v>
+        <v>9.985714285714286</v>
       </c>
       <c r="H10" t="n">
-        <v>0.02326099881093936</v>
+        <v>0.02317228167768793</v>
       </c>
       <c r="I10" t="n">
-        <v>1.385467980295567</v>
+        <v>1.385652973635806</v>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>0.9843505477308294</v>
       </c>
       <c r="K10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -855,30 +887,33 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="D11" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="E11" t="n">
-        <v>0.02586206896551724</v>
+        <v>0.02575107296137339</v>
       </c>
       <c r="F11" t="n">
         <v>0.8571428571428571</v>
       </c>
       <c r="G11" t="n">
-        <v>9.942857142857141</v>
+        <v>9.985714285714286</v>
       </c>
       <c r="H11" t="n">
-        <v>0.02326099881093936</v>
+        <v>0.02317228167768793</v>
       </c>
       <c r="I11" t="n">
-        <v>6.396551724137929</v>
+        <v>6.399141630901286</v>
       </c>
       <c r="J11" t="n">
-        <v>1</v>
+        <v>0.9277286135693216</v>
       </c>
       <c r="K11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -894,30 +929,33 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="D12" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="E12" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.7777777777777777</v>
       </c>
       <c r="G12" t="n">
-        <v>9.022222222222222</v>
+        <v>9.06111111111111</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0268281807372176</v>
+        <v>0.02672732966162574</v>
       </c>
       <c r="I12" t="n">
-        <v>4.112068965517241</v>
+        <v>4.113733905579397</v>
       </c>
       <c r="J12" t="n">
-        <v>1</v>
+        <v>0.9253826530612245</v>
       </c>
       <c r="K12" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -933,108 +971,117 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="D13" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="E13" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="F13" t="n">
         <v>0.35</v>
       </c>
       <c r="G13" t="n">
-        <v>9.022222222222222</v>
+        <v>9.06111111111111</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0268281807372176</v>
+        <v>0.02672732966162574</v>
       </c>
       <c r="I13" t="n">
-        <v>1.478779840848806</v>
+        <v>1.479035985473754</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>0.9731723675385647</v>
       </c>
       <c r="K13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>frozenset({'MS SQL Server'})</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>frozenset({'PostgreSQL'})</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>frozenset({'MS SQL Server'})</t>
-        </is>
-      </c>
       <c r="C14" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="D14" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="E14" t="n">
-        <v>0.03448275862068965</v>
+        <v>0.03433476394849785</v>
       </c>
       <c r="F14" t="n">
-        <v>0.3478260869565217</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="G14" t="n">
-        <v>8.966183574879226</v>
+        <v>9.004830917874395</v>
       </c>
       <c r="H14" t="n">
-        <v>0.03063689060642093</v>
+        <v>0.03052183683619149</v>
       </c>
       <c r="I14" t="n">
-        <v>1.473850574712644</v>
+        <v>8.111587982832614</v>
       </c>
       <c r="J14" t="n">
-        <v>1</v>
+        <v>0.9246651785714286</v>
       </c>
       <c r="K14" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>frozenset({'PostgreSQL'})</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>frozenset({'MS SQL Server'})</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>frozenset({'PostgreSQL'})</t>
-        </is>
-      </c>
       <c r="C15" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="D15" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="E15" t="n">
-        <v>0.03448275862068965</v>
+        <v>0.03433476394849785</v>
       </c>
       <c r="F15" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.3478260869565217</v>
       </c>
       <c r="G15" t="n">
-        <v>8.966183574879226</v>
+        <v>9.004830917874395</v>
       </c>
       <c r="H15" t="n">
-        <v>0.03063689060642093</v>
+        <v>0.03052183683619149</v>
       </c>
       <c r="I15" t="n">
-        <v>8.107758620689651</v>
+        <v>1.474105865522175</v>
       </c>
       <c r="J15" t="n">
-        <v>1</v>
+        <v>0.9863095238095237</v>
       </c>
       <c r="K15" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1050,30 +1097,33 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="D16" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="E16" t="n">
-        <v>0.03448275862068965</v>
+        <v>0.03433476394849785</v>
       </c>
       <c r="F16" t="n">
-        <v>0.7999999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="G16" t="n">
-        <v>8.069565217391304</v>
+        <v>8.104347826086958</v>
       </c>
       <c r="H16" t="n">
-        <v>0.03020957193816885</v>
+        <v>0.03009817826815745</v>
       </c>
       <c r="I16" t="n">
-        <v>4.504310344827585</v>
+        <v>4.506437768240344</v>
       </c>
       <c r="J16" t="n">
-        <v>1</v>
+        <v>0.9159192825112107</v>
       </c>
       <c r="K16" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1089,78 +1139,82 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="D17" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="E17" t="n">
-        <v>0.03448275862068965</v>
+        <v>0.03433476394849785</v>
       </c>
       <c r="F17" t="n">
         <v>0.3478260869565217</v>
       </c>
       <c r="G17" t="n">
-        <v>8.069565217391304</v>
+        <v>8.104347826086956</v>
       </c>
       <c r="H17" t="n">
-        <v>0.03020957193816885</v>
+        <v>0.03009817826815745</v>
       </c>
       <c r="I17" t="n">
-        <v>1.467241379310345</v>
+        <v>1.467525035765379</v>
       </c>
       <c r="J17" t="n">
-        <v>1</v>
+        <v>0.9726190476190476</v>
       </c>
       <c r="K17" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>frozenset({'HyperSQL'})</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>frozenset({'Informix'})</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>frozenset({'HyperSQL'})</t>
-        </is>
-      </c>
       <c r="C18" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="E18" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>0.15625</v>
       </c>
       <c r="G18" t="n">
-        <v>7.25</v>
+        <v>7.28125</v>
       </c>
       <c r="H18" t="n">
-        <v>0.01857907253269917</v>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>0.01851203742931349</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1.159752026704816</v>
       </c>
       <c r="J18" t="n">
         <v>1</v>
       </c>
       <c r="K18" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>frozenset({'IBM DB2'})</t>
+          <t>frozenset({'Informix'})</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1169,22 +1223,22 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="E19" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="F19" t="n">
         <v>1</v>
       </c>
       <c r="G19" t="n">
-        <v>7.25</v>
+        <v>7.28125</v>
       </c>
       <c r="H19" t="n">
-        <v>0.03715814506539834</v>
+        <v>0.01851203742931349</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1192,48 +1246,56 @@
         </is>
       </c>
       <c r="J19" t="n">
-        <v>1</v>
+        <v>0.881578947368421</v>
       </c>
       <c r="K19" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>frozenset({'IBM DB2'})</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>frozenset({'HyperSQL'})</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>frozenset({'Informix'})</t>
-        </is>
-      </c>
       <c r="C20" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="D20" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="E20" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="F20" t="n">
-        <v>0.15625</v>
+        <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>7.249999999999999</v>
+        <v>7.28125</v>
       </c>
       <c r="H20" t="n">
-        <v>0.01857907253269917</v>
-      </c>
-      <c r="I20" t="n">
-        <v>1.159642401021711</v>
+        <v>0.03702407485862698</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
       <c r="J20" t="n">
-        <v>1</v>
+        <v>0.9013452914798207</v>
       </c>
       <c r="K20" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1249,30 +1311,33 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="D21" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="E21" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="F21" t="n">
         <v>0.3125</v>
       </c>
       <c r="G21" t="n">
-        <v>7.249999999999999</v>
+        <v>7.28125</v>
       </c>
       <c r="H21" t="n">
-        <v>0.03715814506539834</v>
+        <v>0.03702407485862698</v>
       </c>
       <c r="I21" t="n">
-        <v>1.391849529780564</v>
+        <v>1.392118611002731</v>
       </c>
       <c r="J21" t="n">
         <v>1</v>
       </c>
       <c r="K21" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1288,30 +1353,33 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="D22" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="E22" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="F22" t="n">
         <v>0.7142857142857143</v>
       </c>
       <c r="G22" t="n">
-        <v>7.204968944099379</v>
+        <v>7.236024844720498</v>
       </c>
       <c r="H22" t="n">
-        <v>0.01856049346016647</v>
+        <v>0.01849361749157288</v>
       </c>
       <c r="I22" t="n">
-        <v>3.15301724137931</v>
+        <v>3.15450643776824</v>
       </c>
       <c r="J22" t="n">
-        <v>1</v>
+        <v>0.888495575221239</v>
       </c>
       <c r="K22" t="n">
+        <v>1</v>
+      </c>
+      <c r="L22" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1327,30 +1395,33 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="D23" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="E23" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="F23" t="n">
         <v>0.2173913043478261</v>
       </c>
       <c r="G23" t="n">
-        <v>7.204968944099378</v>
+        <v>7.236024844720497</v>
       </c>
       <c r="H23" t="n">
-        <v>0.01856049346016647</v>
+        <v>0.01849361749157288</v>
       </c>
       <c r="I23" t="n">
-        <v>1.239224137931034</v>
+        <v>1.239389604196471</v>
       </c>
       <c r="J23" t="n">
-        <v>1</v>
+        <v>0.9561904761904764</v>
       </c>
       <c r="K23" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1366,30 +1437,33 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.05172413793103448</v>
+        <v>0.05150214592274678</v>
       </c>
       <c r="D24" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="E24" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="F24" t="n">
         <v>0.5833333333333334</v>
       </c>
       <c r="G24" t="n">
-        <v>6.766666666666667</v>
+        <v>6.795833333333333</v>
       </c>
       <c r="H24" t="n">
-        <v>0.02571343638525565</v>
+        <v>0.02562213339718912</v>
       </c>
       <c r="I24" t="n">
-        <v>2.193103448275862</v>
+        <v>2.193991416309013</v>
       </c>
       <c r="J24" t="n">
-        <v>1</v>
+        <v>0.8991596638655462</v>
       </c>
       <c r="K24" t="n">
+        <v>1</v>
+      </c>
+      <c r="L24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1405,30 +1479,33 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="D25" t="n">
-        <v>0.05172413793103448</v>
+        <v>0.05150214592274678</v>
       </c>
       <c r="E25" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="F25" t="n">
         <v>0.35</v>
       </c>
       <c r="G25" t="n">
-        <v>6.766666666666667</v>
+        <v>6.795833333333333</v>
       </c>
       <c r="H25" t="n">
-        <v>0.02571343638525565</v>
+        <v>0.02562213339718912</v>
       </c>
       <c r="I25" t="n">
-        <v>1.458885941644562</v>
+        <v>1.459227467811159</v>
       </c>
       <c r="J25" t="n">
-        <v>1</v>
+        <v>0.9329309188464118</v>
       </c>
       <c r="K25" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1444,30 +1521,33 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="D26" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="E26" t="n">
-        <v>0.05603448275862069</v>
+        <v>0.05579399141630902</v>
       </c>
       <c r="F26" t="n">
         <v>0.65</v>
       </c>
       <c r="G26" t="n">
-        <v>6.556521739130435</v>
+        <v>6.584782608695653</v>
       </c>
       <c r="H26" t="n">
-        <v>0.04748810939357907</v>
+        <v>0.04732082005562822</v>
       </c>
       <c r="I26" t="n">
-        <v>2.573891625615764</v>
+        <v>2.575107296137339</v>
       </c>
       <c r="J26" t="n">
-        <v>1</v>
+        <v>0.9277717587576743</v>
       </c>
       <c r="K26" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1483,30 +1563,33 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="D27" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="E27" t="n">
-        <v>0.05603448275862069</v>
+        <v>0.05579399141630902</v>
       </c>
       <c r="F27" t="n">
-        <v>0.5652173913043478</v>
+        <v>0.5652173913043479</v>
       </c>
       <c r="G27" t="n">
-        <v>6.556521739130434</v>
+        <v>6.584782608695653</v>
       </c>
       <c r="H27" t="n">
-        <v>0.04748810939357907</v>
+        <v>0.04732082005562822</v>
       </c>
       <c r="I27" t="n">
-        <v>2.101724137931034</v>
+        <v>2.102575107296138</v>
       </c>
       <c r="J27" t="n">
-        <v>1</v>
+        <v>0.941025641025641</v>
       </c>
       <c r="K27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L27" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1522,30 +1605,33 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.05172413793103448</v>
+        <v>0.05150214592274678</v>
       </c>
       <c r="D28" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="E28" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="F28" t="n">
         <v>0.5833333333333334</v>
       </c>
       <c r="G28" t="n">
-        <v>5.884057971014493</v>
+        <v>5.909420289855073</v>
       </c>
       <c r="H28" t="n">
-        <v>0.02504458977407848</v>
+        <v>0.02495901563852714</v>
       </c>
       <c r="I28" t="n">
-        <v>2.162068965517241</v>
+        <v>2.163090128755365</v>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>0.8758888170652877</v>
       </c>
       <c r="K28" t="n">
+        <v>1</v>
+      </c>
+      <c r="L28" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1561,108 +1647,117 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="D29" t="n">
-        <v>0.05172413793103448</v>
+        <v>0.05150214592274678</v>
       </c>
       <c r="E29" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="F29" t="n">
         <v>0.3043478260869565</v>
       </c>
       <c r="G29" t="n">
-        <v>5.884057971014493</v>
+        <v>5.909420289855073</v>
       </c>
       <c r="H29" t="n">
-        <v>0.02504458977407848</v>
+        <v>0.02495901563852714</v>
       </c>
       <c r="I29" t="n">
-        <v>1.363146551724138</v>
+        <v>1.363465665236052</v>
       </c>
       <c r="J29" t="n">
-        <v>1</v>
+        <v>0.9217687074829931</v>
       </c>
       <c r="K29" t="n">
+        <v>1</v>
+      </c>
+      <c r="L29" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>frozenset({'MS SQL Server'})</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
           <t>frozenset({'H2'})</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>frozenset({'MS SQL Server'})</t>
-        </is>
-      </c>
       <c r="C30" t="n">
-        <v>0.1163793103448276</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="D30" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.1158798283261803</v>
       </c>
       <c r="E30" t="n">
-        <v>0.02586206896551724</v>
+        <v>0.02575107296137339</v>
       </c>
       <c r="F30" t="n">
-        <v>0.2222222222222222</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G30" t="n">
-        <v>5.728395061728396</v>
+        <v>5.753086419753086</v>
       </c>
       <c r="H30" t="n">
-        <v>0.02134735434007135</v>
+        <v>0.02127502809040505</v>
       </c>
       <c r="I30" t="n">
-        <v>1.235837438423645</v>
+        <v>2.652360515021459</v>
       </c>
       <c r="J30" t="n">
-        <v>1</v>
+        <v>0.859375</v>
       </c>
       <c r="K30" t="n">
+        <v>1</v>
+      </c>
+      <c r="L30" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>frozenset({'H2'})</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>frozenset({'MS SQL Server'})</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>frozenset({'H2'})</t>
-        </is>
-      </c>
       <c r="C31" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.1158798283261803</v>
       </c>
       <c r="D31" t="n">
-        <v>0.1163793103448276</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="E31" t="n">
-        <v>0.02586206896551724</v>
+        <v>0.02575107296137339</v>
       </c>
       <c r="F31" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="G31" t="n">
-        <v>5.728395061728395</v>
+        <v>5.753086419753086</v>
       </c>
       <c r="H31" t="n">
-        <v>0.02134735434007135</v>
+        <v>0.02127502809040505</v>
       </c>
       <c r="I31" t="n">
-        <v>2.650862068965517</v>
+        <v>1.236051502145923</v>
       </c>
       <c r="J31" t="n">
-        <v>1</v>
+        <v>0.9344660194174758</v>
       </c>
       <c r="K31" t="n">
+        <v>1</v>
+      </c>
+      <c r="L31" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1678,30 +1773,33 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="D32" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="E32" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="F32" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.7777777777777777</v>
       </c>
       <c r="G32" t="n">
-        <v>5.638888888888889</v>
+        <v>5.663194444444444</v>
       </c>
       <c r="H32" t="n">
-        <v>0.02482164090368609</v>
+        <v>0.02473797638563982</v>
       </c>
       <c r="I32" t="n">
-        <v>3.879310344827586</v>
+        <v>3.881974248927037</v>
       </c>
       <c r="J32" t="n">
-        <v>1</v>
+        <v>0.8565051020408163</v>
       </c>
       <c r="K32" t="n">
+        <v>1</v>
+      </c>
+      <c r="L32" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1717,30 +1815,33 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="D33" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="E33" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="F33" t="n">
         <v>0.21875</v>
       </c>
       <c r="G33" t="n">
-        <v>5.638888888888888</v>
+        <v>5.663194444444444</v>
       </c>
       <c r="H33" t="n">
-        <v>0.02482164090368609</v>
+        <v>0.02473797638563982</v>
       </c>
       <c r="I33" t="n">
-        <v>1.230344827586207</v>
+        <v>1.230557939914163</v>
       </c>
       <c r="J33" t="n">
-        <v>1</v>
+        <v>0.9545131485429994</v>
       </c>
       <c r="K33" t="n">
+        <v>1</v>
+      </c>
+      <c r="L33" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1756,30 +1857,33 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="D34" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="E34" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="F34" t="n">
         <v>0.7142857142857143</v>
       </c>
       <c r="G34" t="n">
-        <v>5.178571428571429</v>
+        <v>5.200892857142858</v>
       </c>
       <c r="H34" t="n">
-        <v>0.01739001189060642</v>
+        <v>0.01733316141391442</v>
       </c>
       <c r="I34" t="n">
-        <v>3.017241379310345</v>
+        <v>3.01931330472103</v>
       </c>
       <c r="J34" t="n">
-        <v>1</v>
+        <v>0.8327433628318583</v>
       </c>
       <c r="K34" t="n">
+        <v>1</v>
+      </c>
+      <c r="L34" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1795,108 +1899,117 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="D35" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="E35" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="F35" t="n">
         <v>0.15625</v>
       </c>
       <c r="G35" t="n">
-        <v>5.178571428571428</v>
+        <v>5.200892857142857</v>
       </c>
       <c r="H35" t="n">
-        <v>0.01739001189060642</v>
+        <v>0.01733316141391442</v>
       </c>
       <c r="I35" t="n">
-        <v>1.149425287356322</v>
+        <v>1.149578763312669</v>
       </c>
       <c r="J35" t="n">
-        <v>1</v>
+        <v>0.9363184079601989</v>
       </c>
       <c r="K35" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>frozenset({'SQLite'})</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
           <t>frozenset({'H2'})</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>frozenset({'SQLite'})</t>
-        </is>
-      </c>
       <c r="C36" t="n">
-        <v>0.1163793103448276</v>
+        <v>0.05150214592274678</v>
       </c>
       <c r="D36" t="n">
-        <v>0.05172413793103448</v>
+        <v>0.1158798283261803</v>
       </c>
       <c r="E36" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="F36" t="n">
-        <v>0.2592592592592593</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="G36" t="n">
-        <v>5.012345679012347</v>
+        <v>5.033950617283951</v>
       </c>
       <c r="H36" t="n">
-        <v>0.02415279429250892</v>
+        <v>0.02407485862697784</v>
       </c>
       <c r="I36" t="n">
-        <v>1.280172413793103</v>
+        <v>2.121888412017168</v>
       </c>
       <c r="J36" t="n">
-        <v>1</v>
+        <v>0.8448610213316097</v>
       </c>
       <c r="K36" t="n">
+        <v>1</v>
+      </c>
+      <c r="L36" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
+          <t>frozenset({'H2'})</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
           <t>frozenset({'SQLite'})</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>frozenset({'H2'})</t>
-        </is>
-      </c>
       <c r="C37" t="n">
-        <v>0.05172413793103448</v>
+        <v>0.1158798283261803</v>
       </c>
       <c r="D37" t="n">
-        <v>0.1163793103448276</v>
+        <v>0.05150214592274678</v>
       </c>
       <c r="E37" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="F37" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.2592592592592592</v>
       </c>
       <c r="G37" t="n">
-        <v>5.012345679012346</v>
+        <v>5.03395061728395</v>
       </c>
       <c r="H37" t="n">
-        <v>0.02415279429250892</v>
+        <v>0.02407485862697784</v>
       </c>
       <c r="I37" t="n">
-        <v>2.120689655172414</v>
+        <v>1.280472103004292</v>
       </c>
       <c r="J37" t="n">
-        <v>1</v>
+        <v>0.9063800277392511</v>
       </c>
       <c r="K37" t="n">
+        <v>1</v>
+      </c>
+      <c r="L37" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1912,30 +2025,33 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="D38" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="E38" t="n">
-        <v>0.05603448275862069</v>
+        <v>0.05579399141630902</v>
       </c>
       <c r="F38" t="n">
         <v>0.65</v>
       </c>
       <c r="G38" t="n">
-        <v>4.7125</v>
+        <v>4.732812500000001</v>
       </c>
       <c r="H38" t="n">
-        <v>0.04414387633769322</v>
+        <v>0.04400523126231834</v>
       </c>
       <c r="I38" t="n">
-        <v>2.463054187192118</v>
+        <v>2.46474555487431</v>
       </c>
       <c r="J38" t="n">
-        <v>1</v>
+        <v>0.8627663416395811</v>
       </c>
       <c r="K38" t="n">
+        <v>1</v>
+      </c>
+      <c r="L38" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1951,76 +2067,82 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="D39" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="E39" t="n">
-        <v>0.05603448275862069</v>
+        <v>0.05579399141630902</v>
       </c>
       <c r="F39" t="n">
         <v>0.40625</v>
       </c>
       <c r="G39" t="n">
-        <v>4.712499999999999</v>
+        <v>4.7328125</v>
       </c>
       <c r="H39" t="n">
-        <v>0.04414387633769322</v>
+        <v>0.04400523126231834</v>
       </c>
       <c r="I39" t="n">
-        <v>1.539019963702359</v>
+        <v>1.53964309916422</v>
       </c>
       <c r="J39" t="n">
-        <v>1</v>
+        <v>0.9142747799464218</v>
       </c>
       <c r="K39" t="n">
+        <v>1</v>
+      </c>
+      <c r="L39" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'MySQL'})</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>frozenset({'IBM DB2'})</t>
+          <t>frozenset({'MS SQL Server'})</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.1163793103448276</v>
+        <v>0.2317596566523605</v>
       </c>
       <c r="D40" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="E40" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="F40" t="n">
-        <v>0.1851851851851852</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="G40" t="n">
-        <v>4.296296296296297</v>
+        <v>4.314814814814815</v>
       </c>
       <c r="H40" t="n">
-        <v>0.01653537455410226</v>
+        <v>0.02967451970012341</v>
       </c>
       <c r="I40" t="n">
-        <v>1.174373040752351</v>
+        <v>1.153648068669528</v>
       </c>
       <c r="J40" t="n">
         <v>1</v>
       </c>
       <c r="K40" t="n">
+        <v>1</v>
+      </c>
+      <c r="L40" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>frozenset({'MS Access'})</t>
+          <t>frozenset({'MS SQL Server'})</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2029,22 +2151,22 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="D41" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.2317596566523605</v>
       </c>
       <c r="E41" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03862660944206009</v>
       </c>
       <c r="F41" t="n">
         <v>1</v>
       </c>
       <c r="G41" t="n">
-        <v>4.296296296296297</v>
+        <v>4.314814814814815</v>
       </c>
       <c r="H41" t="n">
-        <v>0.02314952437574316</v>
+        <v>0.02967451970012341</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
@@ -2052,9 +2174,12 @@
         </is>
       </c>
       <c r="J41" t="n">
-        <v>1</v>
+        <v>0.7991071428571428</v>
       </c>
       <c r="K41" t="n">
+        <v>1</v>
+      </c>
+      <c r="L41" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2070,117 +2195,126 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.2317596566523605</v>
       </c>
       <c r="D42" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="E42" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="F42" t="n">
         <v>0.1851851851851852</v>
       </c>
       <c r="G42" t="n">
-        <v>4.296296296296297</v>
+        <v>4.314814814814815</v>
       </c>
       <c r="H42" t="n">
-        <v>0.03307074910820453</v>
+        <v>0.03297168855569269</v>
       </c>
       <c r="I42" t="n">
-        <v>1.174373040752351</v>
+        <v>1.174600078033555</v>
       </c>
       <c r="J42" t="n">
         <v>1</v>
       </c>
       <c r="K42" t="n">
+        <v>1</v>
+      </c>
+      <c r="L42" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>frozenset({'IBM DB2'})</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
           <t>frozenset({'MySQL'})</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>frozenset({'MS Access'})</t>
-        </is>
-      </c>
       <c r="C43" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="D43" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.2317596566523605</v>
       </c>
       <c r="E43" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="F43" t="n">
-        <v>0.1296296296296297</v>
+        <v>1</v>
       </c>
       <c r="G43" t="n">
-        <v>4.296296296296297</v>
+        <v>4.314814814814815</v>
       </c>
       <c r="H43" t="n">
-        <v>0.02314952437574316</v>
-      </c>
-      <c r="I43" t="n">
-        <v>1.114269992663243</v>
+        <v>0.03297168855569269</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>inf</t>
+        </is>
       </c>
       <c r="J43" t="n">
-        <v>1</v>
+        <v>0.8026905829596414</v>
       </c>
       <c r="K43" t="n">
+        <v>1</v>
+      </c>
+      <c r="L43" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>frozenset({'IBM DB2'})</t>
+          <t>frozenset({'MySQL'})</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'MS Access'})</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.2317596566523605</v>
       </c>
       <c r="D44" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="E44" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="F44" t="n">
-        <v>1</v>
+        <v>0.1296296296296296</v>
       </c>
       <c r="G44" t="n">
-        <v>4.296296296296297</v>
+        <v>4.314814814814815</v>
       </c>
       <c r="H44" t="n">
-        <v>0.03307074910820453</v>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+        <v>0.02308018198898488</v>
+      </c>
+      <c r="I44" t="n">
+        <v>1.114418774541138</v>
       </c>
       <c r="J44" t="n">
         <v>1</v>
       </c>
       <c r="K44" t="n">
+        <v>1</v>
+      </c>
+      <c r="L44" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>frozenset({'MS SQL Server'})</t>
+          <t>frozenset({'MS Access'})</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2189,22 +2323,22 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="D45" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.2317596566523605</v>
       </c>
       <c r="E45" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="F45" t="n">
         <v>1</v>
       </c>
       <c r="G45" t="n">
-        <v>4.296296296296297</v>
+        <v>4.314814814814815</v>
       </c>
       <c r="H45" t="n">
-        <v>0.02976367419738407</v>
+        <v>0.02308018198898488</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
@@ -2212,48 +2346,54 @@
         </is>
       </c>
       <c r="J45" t="n">
-        <v>1</v>
+        <v>0.7920353982300886</v>
       </c>
       <c r="K45" t="n">
+        <v>1</v>
+      </c>
+      <c r="L45" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'H2'})</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>frozenset({'MS SQL Server'})</t>
+          <t>frozenset({'IBM DB2'})</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.1158798283261803</v>
       </c>
       <c r="D46" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="E46" t="n">
-        <v>0.03879310344827586</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="F46" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.1851851851851852</v>
       </c>
       <c r="G46" t="n">
-        <v>4.296296296296297</v>
+        <v>4.314814814814815</v>
       </c>
       <c r="H46" t="n">
-        <v>0.02976367419738407</v>
+        <v>0.01648584427784634</v>
       </c>
       <c r="I46" t="n">
-        <v>1.153448275862069</v>
+        <v>1.174600078033555</v>
       </c>
       <c r="J46" t="n">
-        <v>1</v>
+        <v>0.8689320388349516</v>
       </c>
       <c r="K46" t="n">
+        <v>1</v>
+      </c>
+      <c r="L46" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2269,108 +2409,117 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="D47" t="n">
-        <v>0.1163793103448276</v>
+        <v>0.1158798283261803</v>
       </c>
       <c r="E47" t="n">
-        <v>0.02155172413793104</v>
+        <v>0.02145922746781116</v>
       </c>
       <c r="F47" t="n">
         <v>0.5</v>
       </c>
       <c r="G47" t="n">
-        <v>4.296296296296297</v>
+        <v>4.314814814814815</v>
       </c>
       <c r="H47" t="n">
-        <v>0.01653537455410226</v>
+        <v>0.01648584427784634</v>
       </c>
       <c r="I47" t="n">
-        <v>1.767241379310345</v>
+        <v>1.768240343347639</v>
       </c>
       <c r="J47" t="n">
-        <v>1</v>
+        <v>0.8026905829596414</v>
       </c>
       <c r="K47" t="n">
+        <v>1</v>
+      </c>
+      <c r="L47" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
+          <t>frozenset({'PostgreSQL'})</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
           <t>frozenset({'HyperSQL'})</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>frozenset({'PostgreSQL'})</t>
-        </is>
-      </c>
       <c r="C48" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="D48" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="E48" t="n">
-        <v>0.05603448275862069</v>
+        <v>0.05579399141630902</v>
       </c>
       <c r="F48" t="n">
-        <v>0.40625</v>
+        <v>0.5652173913043479</v>
       </c>
       <c r="G48" t="n">
-        <v>4.097826086956522</v>
+        <v>4.115489130434783</v>
       </c>
       <c r="H48" t="n">
-        <v>0.0423602853745541</v>
+        <v>0.04223691723921973</v>
       </c>
       <c r="I48" t="n">
-        <v>1.517241379310345</v>
+        <v>1.98412017167382</v>
       </c>
       <c r="J48" t="n">
-        <v>1</v>
+        <v>0.8399267399267399</v>
       </c>
       <c r="K48" t="n">
+        <v>1</v>
+      </c>
+      <c r="L48" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>frozenset({'HyperSQL'})</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
           <t>frozenset({'PostgreSQL'})</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>frozenset({'HyperSQL'})</t>
-        </is>
-      </c>
       <c r="C49" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="D49" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="E49" t="n">
-        <v>0.05603448275862069</v>
+        <v>0.05579399141630902</v>
       </c>
       <c r="F49" t="n">
-        <v>0.5652173913043478</v>
+        <v>0.40625</v>
       </c>
       <c r="G49" t="n">
-        <v>4.097826086956522</v>
+        <v>4.115489130434783</v>
       </c>
       <c r="H49" t="n">
-        <v>0.0423602853745541</v>
+        <v>0.04223691723921973</v>
       </c>
       <c r="I49" t="n">
-        <v>1.982758620689655</v>
+        <v>1.517957985091484</v>
       </c>
       <c r="J49" t="n">
-        <v>1</v>
+        <v>0.8775353999234596</v>
       </c>
       <c r="K49" t="n">
+        <v>1</v>
+      </c>
+      <c r="L49" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2386,30 +2535,33 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="D50" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.2317596566523605</v>
       </c>
       <c r="E50" t="n">
-        <v>0.09051724137931035</v>
+        <v>0.09012875536480687</v>
       </c>
       <c r="F50" t="n">
-        <v>0.9130434782608695</v>
+        <v>0.9130434782608696</v>
       </c>
       <c r="G50" t="n">
-        <v>3.922705314009662</v>
+        <v>3.939613526570048</v>
       </c>
       <c r="H50" t="n">
-        <v>0.06744203329369798</v>
+        <v>0.06725119269096871</v>
       </c>
       <c r="I50" t="n">
-        <v>8.823275862068961</v>
+        <v>8.83476394849786</v>
       </c>
       <c r="J50" t="n">
-        <v>1</v>
+        <v>0.827891156462585</v>
       </c>
       <c r="K50" t="n">
+        <v>1</v>
+      </c>
+      <c r="L50" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2425,30 +2577,33 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.2317596566523605</v>
       </c>
       <c r="D51" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="E51" t="n">
-        <v>0.09051724137931035</v>
+        <v>0.09012875536480687</v>
       </c>
       <c r="F51" t="n">
         <v>0.3888888888888889</v>
       </c>
       <c r="G51" t="n">
-        <v>3.922705314009662</v>
+        <v>3.939613526570048</v>
       </c>
       <c r="H51" t="n">
-        <v>0.06744203329369798</v>
+        <v>0.06725119269096871</v>
       </c>
       <c r="I51" t="n">
-        <v>1.474137931034483</v>
+        <v>1.47483417869684</v>
       </c>
       <c r="J51" t="n">
-        <v>1</v>
+        <v>0.9712689545091782</v>
       </c>
       <c r="K51" t="n">
+        <v>1</v>
+      </c>
+      <c r="L51" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2464,30 +2619,33 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.1163793103448276</v>
+        <v>0.1158798283261803</v>
       </c>
       <c r="D52" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="E52" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="F52" t="n">
         <v>0.3703703703703704</v>
       </c>
       <c r="G52" t="n">
-        <v>3.735909822866345</v>
+        <v>3.752012882447666</v>
       </c>
       <c r="H52" t="n">
-        <v>0.03156584423305589</v>
+        <v>0.03147967359870324</v>
       </c>
       <c r="I52" t="n">
-        <v>1.43078093306288</v>
+        <v>1.431456702852815</v>
       </c>
       <c r="J52" t="n">
-        <v>1</v>
+        <v>0.8296116504854371</v>
       </c>
       <c r="K52" t="n">
+        <v>1</v>
+      </c>
+      <c r="L52" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2503,30 +2661,33 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.09913793103448276</v>
+        <v>0.09871244635193133</v>
       </c>
       <c r="D53" t="n">
-        <v>0.1163793103448276</v>
+        <v>0.1158798283261803</v>
       </c>
       <c r="E53" t="n">
-        <v>0.04310344827586207</v>
+        <v>0.04291845493562232</v>
       </c>
       <c r="F53" t="n">
         <v>0.4347826086956522</v>
       </c>
       <c r="G53" t="n">
-        <v>3.735909822866345</v>
+        <v>3.752012882447665</v>
       </c>
       <c r="H53" t="n">
-        <v>0.03156584423305589</v>
+        <v>0.03147967359870324</v>
       </c>
       <c r="I53" t="n">
-        <v>1.563328912466843</v>
+        <v>1.564212611422912</v>
       </c>
       <c r="J53" t="n">
-        <v>1</v>
+        <v>0.813809523809524</v>
       </c>
       <c r="K53" t="n">
+        <v>1</v>
+      </c>
+      <c r="L53" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2542,30 +2703,33 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="D54" t="n">
-        <v>0.05172413793103448</v>
+        <v>0.05150214592274678</v>
       </c>
       <c r="E54" t="n">
-        <v>0.02586206896551724</v>
+        <v>0.02575107296137339</v>
       </c>
       <c r="F54" t="n">
         <v>0.1875</v>
       </c>
       <c r="G54" t="n">
-        <v>3.625</v>
+        <v>3.640625</v>
       </c>
       <c r="H54" t="n">
-        <v>0.01872770511296076</v>
+        <v>0.01867781686897898</v>
       </c>
       <c r="I54" t="n">
-        <v>1.16710875331565</v>
+        <v>1.167381974248927</v>
       </c>
       <c r="J54" t="n">
-        <v>1</v>
+        <v>0.8407960199004975</v>
       </c>
       <c r="K54" t="n">
+        <v>1</v>
+      </c>
+      <c r="L54" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2581,30 +2745,33 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0.05172413793103448</v>
+        <v>0.05150214592274678</v>
       </c>
       <c r="D55" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="E55" t="n">
-        <v>0.02586206896551724</v>
+        <v>0.02575107296137339</v>
       </c>
       <c r="F55" t="n">
         <v>0.5</v>
       </c>
       <c r="G55" t="n">
-        <v>3.625</v>
+        <v>3.640625</v>
       </c>
       <c r="H55" t="n">
-        <v>0.01872770511296076</v>
+        <v>0.01867781686897898</v>
       </c>
       <c r="I55" t="n">
-        <v>1.724137931034483</v>
+        <v>1.725321888412017</v>
       </c>
       <c r="J55" t="n">
-        <v>1</v>
+        <v>0.7647058823529412</v>
       </c>
       <c r="K55" t="n">
+        <v>1</v>
+      </c>
+      <c r="L55" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2620,30 +2787,33 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="D56" t="n">
-        <v>0.1163793103448276</v>
+        <v>0.1158798283261803</v>
       </c>
       <c r="E56" t="n">
-        <v>0.03448275862068965</v>
+        <v>0.03433476394849785</v>
       </c>
       <c r="F56" t="n">
         <v>0.4</v>
       </c>
       <c r="G56" t="n">
-        <v>3.437037037037037</v>
+        <v>3.451851851851852</v>
       </c>
       <c r="H56" t="n">
-        <v>0.0244500594530321</v>
+        <v>0.02438799756856822</v>
       </c>
       <c r="I56" t="n">
-        <v>1.472701149425287</v>
+        <v>1.473533619456366</v>
       </c>
       <c r="J56" t="n">
-        <v>1</v>
+        <v>0.7769953051643191</v>
       </c>
       <c r="K56" t="n">
+        <v>1</v>
+      </c>
+      <c r="L56" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2659,108 +2829,117 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0.1163793103448276</v>
+        <v>0.1158798283261803</v>
       </c>
       <c r="D57" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="E57" t="n">
-        <v>0.03448275862068965</v>
+        <v>0.03433476394849785</v>
       </c>
       <c r="F57" t="n">
         <v>0.2962962962962963</v>
       </c>
       <c r="G57" t="n">
-        <v>3.437037037037037</v>
+        <v>3.451851851851852</v>
       </c>
       <c r="H57" t="n">
-        <v>0.0244500594530321</v>
+        <v>0.02438799756856822</v>
       </c>
       <c r="I57" t="n">
-        <v>1.298548094373866</v>
+        <v>1.29907386491981</v>
       </c>
       <c r="J57" t="n">
-        <v>1</v>
+        <v>0.8033980582524273</v>
       </c>
       <c r="K57" t="n">
+        <v>1</v>
+      </c>
+      <c r="L57" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
+          <t>frozenset({'MySQL'})</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
           <t>frozenset({'Oracle'})</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>frozenset({'MySQL'})</t>
-        </is>
-      </c>
       <c r="C58" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.2317596566523605</v>
       </c>
       <c r="D58" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="E58" t="n">
-        <v>0.06465517241379311</v>
+        <v>0.06437768240343347</v>
       </c>
       <c r="F58" t="n">
-        <v>0.75</v>
+        <v>0.2777777777777778</v>
       </c>
       <c r="G58" t="n">
-        <v>3.222222222222222</v>
+        <v>3.236111111111111</v>
       </c>
       <c r="H58" t="n">
-        <v>0.04458977407847801</v>
+        <v>0.0444841496435742</v>
       </c>
       <c r="I58" t="n">
-        <v>3.068965517241379</v>
+        <v>1.265764278639815</v>
       </c>
       <c r="J58" t="n">
-        <v>1</v>
+        <v>0.8994413407821229</v>
       </c>
       <c r="K58" t="n">
+        <v>1</v>
+      </c>
+      <c r="L58" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>frozenset({'MySQL'})</t>
+          <t>frozenset({'H2'})</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>frozenset({'Oracle'})</t>
+          <t>frozenset({'HyperSQL'})</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.1158798283261803</v>
       </c>
       <c r="D59" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="E59" t="n">
-        <v>0.06465517241379311</v>
+        <v>0.05150214592274678</v>
       </c>
       <c r="F59" t="n">
-        <v>0.2777777777777778</v>
+        <v>0.4444444444444445</v>
       </c>
       <c r="G59" t="n">
-        <v>3.222222222222222</v>
+        <v>3.236111111111111</v>
       </c>
       <c r="H59" t="n">
-        <v>0.04458977407847801</v>
+        <v>0.03558731971485937</v>
       </c>
       <c r="I59" t="n">
-        <v>1.26525198938992</v>
+        <v>1.552789699570815</v>
       </c>
       <c r="J59" t="n">
-        <v>1</v>
+        <v>0.7815533980582525</v>
       </c>
       <c r="K59" t="n">
+        <v>1</v>
+      </c>
+      <c r="L59" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2776,147 +2955,159 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="D60" t="n">
-        <v>0.1163793103448276</v>
+        <v>0.1158798283261803</v>
       </c>
       <c r="E60" t="n">
-        <v>0.05172413793103448</v>
+        <v>0.05150214592274678</v>
       </c>
       <c r="F60" t="n">
         <v>0.375</v>
       </c>
       <c r="G60" t="n">
-        <v>3.222222222222222</v>
+        <v>3.236111111111111</v>
       </c>
       <c r="H60" t="n">
-        <v>0.0356718192627824</v>
+        <v>0.03558731971485937</v>
       </c>
       <c r="I60" t="n">
-        <v>1.413793103448276</v>
+        <v>1.414592274678112</v>
       </c>
       <c r="J60" t="n">
-        <v>1</v>
+        <v>0.8009950248756219</v>
       </c>
       <c r="K60" t="n">
+        <v>1</v>
+      </c>
+      <c r="L60" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>frozenset({'H2'})</t>
+          <t>frozenset({'Oracle'})</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>frozenset({'HyperSQL'})</t>
+          <t>frozenset({'MySQL'})</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.1163793103448276</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="D61" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.2317596566523605</v>
       </c>
       <c r="E61" t="n">
-        <v>0.05172413793103448</v>
+        <v>0.06437768240343347</v>
       </c>
       <c r="F61" t="n">
-        <v>0.4444444444444445</v>
+        <v>0.75</v>
       </c>
       <c r="G61" t="n">
-        <v>3.222222222222222</v>
+        <v>3.236111111111111</v>
       </c>
       <c r="H61" t="n">
-        <v>0.0356718192627824</v>
+        <v>0.0444841496435742</v>
       </c>
       <c r="I61" t="n">
-        <v>1.551724137931034</v>
+        <v>3.072961373390558</v>
       </c>
       <c r="J61" t="n">
-        <v>1</v>
+        <v>0.7558685446009389</v>
       </c>
       <c r="K61" t="n">
+        <v>1</v>
+      </c>
+      <c r="L61" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
+          <t>frozenset({'H2'})</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
           <t>frozenset({'MySQL'})</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>frozenset({'H2'})</t>
-        </is>
-      </c>
       <c r="C62" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.1158798283261803</v>
       </c>
       <c r="D62" t="n">
-        <v>0.1163793103448276</v>
+        <v>0.2317596566523605</v>
       </c>
       <c r="E62" t="n">
-        <v>0.07327586206896551</v>
+        <v>0.07296137339055794</v>
       </c>
       <c r="F62" t="n">
-        <v>0.3148148148148148</v>
+        <v>0.6296296296296297</v>
       </c>
       <c r="G62" t="n">
-        <v>2.705075445816186</v>
+        <v>2.716735253772291</v>
       </c>
       <c r="H62" t="n">
-        <v>0.04618757431629013</v>
+        <v>0.04610510416474793</v>
       </c>
       <c r="I62" t="n">
-        <v>1.289608574091333</v>
+        <v>2.074248927038627</v>
       </c>
       <c r="J62" t="n">
-        <v>1</v>
+        <v>0.7147344374643062</v>
       </c>
       <c r="K62" t="n">
+        <v>1</v>
+      </c>
+      <c r="L62" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
+          <t>frozenset({'MySQL'})</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
           <t>frozenset({'H2'})</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>frozenset({'MySQL'})</t>
-        </is>
-      </c>
       <c r="C63" t="n">
-        <v>0.1163793103448276</v>
+        <v>0.2317596566523605</v>
       </c>
       <c r="D63" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.1158798283261803</v>
       </c>
       <c r="E63" t="n">
-        <v>0.07327586206896551</v>
+        <v>0.07296137339055794</v>
       </c>
       <c r="F63" t="n">
-        <v>0.6296296296296295</v>
+        <v>0.3148148148148148</v>
       </c>
       <c r="G63" t="n">
-        <v>2.705075445816186</v>
+        <v>2.716735253772291</v>
       </c>
       <c r="H63" t="n">
-        <v>0.04618757431629013</v>
+        <v>0.04610510416474793</v>
       </c>
       <c r="I63" t="n">
-        <v>2.07155172413793</v>
+        <v>1.290337547848277</v>
       </c>
       <c r="J63" t="n">
-        <v>1</v>
+        <v>0.8225435425566877</v>
       </c>
       <c r="K63" t="n">
+        <v>1</v>
+      </c>
+      <c r="L63" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2932,30 +3123,33 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.2317596566523605</v>
       </c>
       <c r="D64" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="E64" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="F64" t="n">
         <v>0.3703703703703704</v>
       </c>
       <c r="G64" t="n">
-        <v>2.685185185185186</v>
+        <v>2.69675925925926</v>
       </c>
       <c r="H64" t="n">
-        <v>0.05410225921521998</v>
+        <v>0.0540072574554698</v>
       </c>
       <c r="I64" t="n">
-        <v>1.369168356997972</v>
+        <v>1.370108558444837</v>
       </c>
       <c r="J64" t="n">
-        <v>1</v>
+        <v>0.8189944134078213</v>
       </c>
       <c r="K64" t="n">
+        <v>1</v>
+      </c>
+      <c r="L64" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2971,108 +3165,117 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.1379310344827586</v>
+        <v>0.1373390557939914</v>
       </c>
       <c r="D65" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.2317596566523605</v>
       </c>
       <c r="E65" t="n">
-        <v>0.08620689655172414</v>
+        <v>0.08583690987124463</v>
       </c>
       <c r="F65" t="n">
         <v>0.625</v>
       </c>
       <c r="G65" t="n">
-        <v>2.685185185185185</v>
+        <v>2.69675925925926</v>
       </c>
       <c r="H65" t="n">
-        <v>0.05410225921521998</v>
+        <v>0.0540072574554698</v>
       </c>
       <c r="I65" t="n">
-        <v>2.045977011494253</v>
+        <v>2.048640915593705</v>
       </c>
       <c r="J65" t="n">
-        <v>1</v>
+        <v>0.7293532338308458</v>
       </c>
       <c r="K65" t="n">
+        <v>1</v>
+      </c>
+      <c r="L65" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
+          <t>frozenset({'SQLite'})</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
           <t>frozenset({'MySQL'})</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>frozenset({'SQLite'})</t>
-        </is>
-      </c>
       <c r="C66" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.05150214592274678</v>
       </c>
       <c r="D66" t="n">
-        <v>0.05172413793103448</v>
+        <v>0.2317596566523605</v>
       </c>
       <c r="E66" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="F66" t="n">
-        <v>0.1296296296296297</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="G66" t="n">
-        <v>2.506172839506173</v>
+        <v>2.516975308641975</v>
       </c>
       <c r="H66" t="n">
-        <v>0.01813317479191439</v>
+        <v>0.01810679879902006</v>
       </c>
       <c r="I66" t="n">
-        <v>1.089508437270726</v>
+        <v>1.843776824034335</v>
       </c>
       <c r="J66" t="n">
-        <v>1</v>
+        <v>0.6354234001292824</v>
       </c>
       <c r="K66" t="n">
+        <v>1</v>
+      </c>
+      <c r="L66" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
+          <t>frozenset({'MySQL'})</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
           <t>frozenset({'SQLite'})</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>frozenset({'MySQL'})</t>
-        </is>
-      </c>
       <c r="C67" t="n">
-        <v>0.05172413793103448</v>
+        <v>0.2317596566523605</v>
       </c>
       <c r="D67" t="n">
-        <v>0.2327586206896552</v>
+        <v>0.05150214592274678</v>
       </c>
       <c r="E67" t="n">
-        <v>0.03017241379310345</v>
+        <v>0.03004291845493562</v>
       </c>
       <c r="F67" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.1296296296296296</v>
       </c>
       <c r="G67" t="n">
-        <v>2.506172839506173</v>
+        <v>2.516975308641975</v>
       </c>
       <c r="H67" t="n">
-        <v>0.01813317479191439</v>
+        <v>0.01810679879902006</v>
       </c>
       <c r="I67" t="n">
-        <v>1.841379310344828</v>
+        <v>1.089763491918546</v>
       </c>
       <c r="J67" t="n">
-        <v>1</v>
+        <v>0.7845171588188349</v>
       </c>
       <c r="K67" t="n">
+        <v>1</v>
+      </c>
+      <c r="L67" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>